<commit_message>
Provided the estimation for CRs
</commit_message>
<xml_diff>
--- a/requirements/MOSIP_Requirements Change_Tracker_18Dec18_Updated.xlsx
+++ b/requirements/MOSIP_Requirements Change_Tracker_18Dec18_Updated.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\m1032103\Desktop\ReviewMails\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MOSIP_GIT_HUB\requirements\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{39E9D3FD-69AC-4306-BB4E-49D2E9F36C9D}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7050" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7050"/>
   </bookViews>
   <sheets>
     <sheet name="MOSIP_QueryLog_External" sheetId="5" r:id="rId1"/>
@@ -20,9 +19,9 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">MOSIP_QueryLog_External!$A$2:$O$70</definedName>
   </definedNames>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="162913"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId4"/>
+    <pivotCache cacheId="1" r:id="rId4"/>
   </pivotCaches>
   <fileRecoveryPr autoRecover="0"/>
   <extLst>
@@ -34,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="665" uniqueCount="214">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="667" uniqueCount="216">
   <si>
     <t>MOSIP - Requirements Change Log</t>
   </si>
@@ -2329,11 +2328,24 @@
 3. Once a TSP is authorized they should ideally have a self-service (TSP Portal) mechanism to get their keys, and regenerate them on need basis. In the absence of a Self-Service portal, it should be possible for the admin to generate the key and email it to the TSP. This can be done as part of the approval process, as well as on an ad hoc basis when the key needs to be replaced</t>
     </r>
   </si>
+  <si>
+    <t xml:space="preserve">Statsus Updated to Exported for the exported.
+FilePath should be a configurable one.
+Offline only export should work.
+Serice changes, UI changes. 
+EOD Approval Screen On/Off. 
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Pre-Reg Sync/Batch Job Changes
+2. Multi-lingual changes 
+3. ID object based strucutre changes </t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -2705,7 +2717,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
       <tableStyleElement type="wholeTable" dxfId="1"/>
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
@@ -2722,7 +2734,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="MINDTREE" refreshedDate="43448.660082060182" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="64" xr:uid="{274F372A-FD82-4F30-95A5-944920002719}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="MINDTREE" refreshedDate="43448.660082060182" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="64">
   <cacheSource type="worksheet">
     <worksheetSource ref="A2:O68" sheet="MOSIP_QueryLog_External"/>
   </cacheSource>
@@ -3883,7 +3895,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{5CC952D1-97B4-4C44-9B0D-589F215B138A}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:C11" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="15">
     <pivotField dataField="1" showAll="0"/>
@@ -4231,36 +4243,36 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
   <dimension ref="A1:O70"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:O1"/>
+      <pane ySplit="2" topLeftCell="A68" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D70" sqref="D70"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="20.28515625" defaultRowHeight="14.25" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="20.26953125" defaultRowHeight="14" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="6.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.453125" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14" style="2" customWidth="1"/>
-    <col min="3" max="3" width="30.42578125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="15.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.7109375" style="3" customWidth="1"/>
-    <col min="6" max="6" width="71.140625" style="3" customWidth="1"/>
-    <col min="7" max="7" width="13.28515625" style="22" customWidth="1"/>
-    <col min="8" max="8" width="44.42578125" style="3" customWidth="1"/>
-    <col min="9" max="9" width="9.28515625" style="3" customWidth="1"/>
-    <col min="10" max="10" width="20.85546875" style="3" customWidth="1"/>
-    <col min="11" max="11" width="12.28515625" style="3" customWidth="1"/>
-    <col min="12" max="12" width="12.5703125" style="3" customWidth="1"/>
-    <col min="13" max="13" width="12.7109375" style="37" hidden="1" customWidth="1"/>
-    <col min="14" max="14" width="15.85546875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="30.453125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="15.7265625" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.7265625" style="3" customWidth="1"/>
+    <col min="6" max="6" width="71.1796875" style="3" customWidth="1"/>
+    <col min="7" max="7" width="13.26953125" style="22" customWidth="1"/>
+    <col min="8" max="8" width="44.453125" style="3" customWidth="1"/>
+    <col min="9" max="9" width="9.26953125" style="3" customWidth="1"/>
+    <col min="10" max="10" width="20.81640625" style="3" customWidth="1"/>
+    <col min="11" max="11" width="12.26953125" style="3" customWidth="1"/>
+    <col min="12" max="12" width="12.54296875" style="3" customWidth="1"/>
+    <col min="13" max="13" width="12.7265625" style="37" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="15.81640625" style="2" customWidth="1"/>
     <col min="15" max="15" width="35" style="3" customWidth="1"/>
-    <col min="16" max="16384" width="20.28515625" style="14"/>
+    <col min="16" max="16384" width="20.26953125" style="14"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="48" t="s">
         <v>0</v>
       </c>
@@ -4279,7 +4291,7 @@
       <c r="N1" s="49"/>
       <c r="O1" s="50"/>
     </row>
-    <row r="2" spans="1:15" ht="57" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" ht="42" x14ac:dyDescent="0.35">
       <c r="A2" s="24" t="s">
         <v>1</v>
       </c>
@@ -4326,7 +4338,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:15" s="4" customFormat="1" ht="128.25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" s="4" customFormat="1" ht="112" x14ac:dyDescent="0.35">
       <c r="A3" s="5">
         <v>1</v>
       </c>
@@ -4373,7 +4385,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:15" s="4" customFormat="1" ht="57" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" s="4" customFormat="1" ht="56" x14ac:dyDescent="0.35">
       <c r="A4" s="5">
         <v>2</v>
       </c>
@@ -4420,7 +4432,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:15" s="4" customFormat="1" ht="71.25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" s="4" customFormat="1" ht="70" x14ac:dyDescent="0.35">
       <c r="A5" s="5">
         <v>3</v>
       </c>
@@ -4467,7 +4479,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:15" s="4" customFormat="1" ht="57" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" s="4" customFormat="1" ht="56" x14ac:dyDescent="0.35">
       <c r="A6" s="5">
         <v>4</v>
       </c>
@@ -4514,7 +4526,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:15" s="1" customFormat="1" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:15" s="1" customFormat="1" ht="42" x14ac:dyDescent="0.3">
       <c r="A7" s="5">
         <v>5</v>
       </c>
@@ -4560,7 +4572,7 @@
       </c>
       <c r="O7" s="28"/>
     </row>
-    <row r="8" spans="1:15" s="1" customFormat="1" ht="57" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:15" s="1" customFormat="1" ht="56" x14ac:dyDescent="0.3">
       <c r="A8" s="5">
         <v>6</v>
       </c>
@@ -4605,7 +4617,7 @@
       </c>
       <c r="O8" s="28"/>
     </row>
-    <row r="9" spans="1:15" s="1" customFormat="1" ht="213.75" hidden="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:15" s="1" customFormat="1" ht="210" hidden="1" x14ac:dyDescent="0.3">
       <c r="A9" s="5">
         <v>7</v>
       </c>
@@ -4649,7 +4661,7 @@
       </c>
       <c r="O9" s="28"/>
     </row>
-    <row r="10" spans="1:15" s="1" customFormat="1" ht="71.25" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:15" s="1" customFormat="1" ht="56" x14ac:dyDescent="0.3">
       <c r="A10" s="5">
         <v>8</v>
       </c>
@@ -4696,7 +4708,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="11" spans="1:15" s="1" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:15" s="1" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="5">
         <v>9</v>
       </c>
@@ -4743,7 +4755,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="12" spans="1:15" s="1" customFormat="1" ht="114" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:15" s="1" customFormat="1" ht="112" x14ac:dyDescent="0.3">
       <c r="A12" s="5">
         <v>10</v>
       </c>
@@ -4790,7 +4802,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="13" spans="1:15" s="4" customFormat="1" ht="171" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" s="4" customFormat="1" ht="154" x14ac:dyDescent="0.35">
       <c r="A13" s="5">
         <v>11</v>
       </c>
@@ -4837,7 +4849,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="14" spans="1:15" s="1" customFormat="1" ht="114" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:15" s="1" customFormat="1" ht="98" x14ac:dyDescent="0.3">
       <c r="A14" s="5">
         <v>12</v>
       </c>
@@ -4882,7 +4894,7 @@
       </c>
       <c r="O14" s="28"/>
     </row>
-    <row r="15" spans="1:15" s="4" customFormat="1" ht="114" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" s="4" customFormat="1" ht="98" x14ac:dyDescent="0.35">
       <c r="A15" s="5">
         <v>13</v>
       </c>
@@ -4929,7 +4941,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="16" spans="1:15" s="1" customFormat="1" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:15" s="1" customFormat="1" ht="42" x14ac:dyDescent="0.3">
       <c r="A16" s="5">
         <v>14</v>
       </c>
@@ -4973,7 +4985,7 @@
       </c>
       <c r="O16" s="28"/>
     </row>
-    <row r="17" spans="1:15" s="4" customFormat="1" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" s="4" customFormat="1" ht="42" x14ac:dyDescent="0.35">
       <c r="A17" s="5">
         <v>15</v>
       </c>
@@ -5017,7 +5029,7 @@
       </c>
       <c r="O17" s="28"/>
     </row>
-    <row r="18" spans="1:15" ht="99.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" ht="84" x14ac:dyDescent="0.35">
       <c r="A18" s="5">
         <v>16</v>
       </c>
@@ -5064,7 +5076,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="19" spans="1:15" ht="99.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" ht="84" x14ac:dyDescent="0.35">
       <c r="A19" s="5">
         <v>17</v>
       </c>
@@ -5111,7 +5123,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="20" spans="1:15" ht="99.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" ht="84" x14ac:dyDescent="0.35">
       <c r="A20" s="5">
         <v>18</v>
       </c>
@@ -5158,7 +5170,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="21" spans="1:15" ht="85.5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" ht="84" x14ac:dyDescent="0.35">
       <c r="A21" s="5">
         <v>19</v>
       </c>
@@ -5203,7 +5215,7 @@
       </c>
       <c r="O21" s="28"/>
     </row>
-    <row r="22" spans="1:15" ht="99.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" ht="84" x14ac:dyDescent="0.35">
       <c r="A22" s="5">
         <v>20</v>
       </c>
@@ -5248,7 +5260,7 @@
       </c>
       <c r="O22" s="28"/>
     </row>
-    <row r="23" spans="1:15" ht="99.75" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" ht="84" x14ac:dyDescent="0.35">
       <c r="A23" s="5">
         <v>21</v>
       </c>
@@ -5295,7 +5307,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="24" spans="1:15" ht="85.5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" ht="84" x14ac:dyDescent="0.35">
       <c r="A24" s="5">
         <v>22</v>
       </c>
@@ -5342,7 +5354,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="25" spans="1:15" ht="85.5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" ht="84" x14ac:dyDescent="0.35">
       <c r="A25" s="5">
         <v>23</v>
       </c>
@@ -5387,7 +5399,7 @@
       </c>
       <c r="O25" s="28"/>
     </row>
-    <row r="26" spans="1:15" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" ht="42" x14ac:dyDescent="0.35">
       <c r="A26" s="5">
         <v>24</v>
       </c>
@@ -5432,7 +5444,7 @@
       </c>
       <c r="O26" s="20"/>
     </row>
-    <row r="27" spans="1:15" ht="85.5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" ht="70" x14ac:dyDescent="0.35">
       <c r="A27" s="5">
         <v>25</v>
       </c>
@@ -5479,7 +5491,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="28" spans="1:15" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" ht="42" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="5">
         <v>26</v>
       </c>
@@ -5517,7 +5529,7 @@
       </c>
       <c r="O28" s="42"/>
     </row>
-    <row r="29" spans="1:15" s="11" customFormat="1" ht="85.5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" s="11" customFormat="1" ht="84" x14ac:dyDescent="0.35">
       <c r="A29" s="5">
         <v>27</v>
       </c>
@@ -5564,7 +5576,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="30" spans="1:15" s="11" customFormat="1" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15" s="11" customFormat="1" ht="42" x14ac:dyDescent="0.35">
       <c r="A30" s="5">
         <v>28</v>
       </c>
@@ -5611,7 +5623,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="31" spans="1:15" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:15" ht="42" x14ac:dyDescent="0.35">
       <c r="A31" s="5">
         <v>29</v>
       </c>
@@ -5656,7 +5668,7 @@
       </c>
       <c r="O31" s="20"/>
     </row>
-    <row r="32" spans="1:15" ht="128.25" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:15" ht="126" x14ac:dyDescent="0.35">
       <c r="A32" s="5">
         <v>30</v>
       </c>
@@ -5704,7 +5716,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="33" spans="1:15" ht="85.5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:15" ht="70" x14ac:dyDescent="0.35">
       <c r="A33" s="5">
         <v>31</v>
       </c>
@@ -5751,7 +5763,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="34" spans="1:15" ht="142.5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:15" ht="140" x14ac:dyDescent="0.35">
       <c r="A34" s="5">
         <v>32</v>
       </c>
@@ -5799,7 +5811,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="35" spans="1:15" ht="71.25" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:15" ht="70" x14ac:dyDescent="0.35">
       <c r="A35" s="5">
         <v>33</v>
       </c>
@@ -5847,7 +5859,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="36" spans="1:15" ht="36" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:15" ht="36" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" s="5">
         <v>34</v>
       </c>
@@ -5891,7 +5903,7 @@
       </c>
       <c r="O36" s="42"/>
     </row>
-    <row r="37" spans="1:15" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:15" ht="28" hidden="1" x14ac:dyDescent="0.35">
       <c r="A37" s="5">
         <v>35</v>
       </c>
@@ -5935,7 +5947,7 @@
       </c>
       <c r="O37" s="42"/>
     </row>
-    <row r="38" spans="1:15" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:15" ht="28" hidden="1" x14ac:dyDescent="0.35">
       <c r="A38" s="5">
         <v>36</v>
       </c>
@@ -5979,7 +5991,7 @@
       </c>
       <c r="O38" s="42"/>
     </row>
-    <row r="39" spans="1:15" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:15" ht="28" hidden="1" x14ac:dyDescent="0.35">
       <c r="A39" s="5">
         <v>37</v>
       </c>
@@ -6023,7 +6035,7 @@
       </c>
       <c r="O39" s="42"/>
     </row>
-    <row r="40" spans="1:15" ht="256.5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:15" ht="252" x14ac:dyDescent="0.35">
       <c r="A40" s="5">
         <v>38</v>
       </c>
@@ -6070,7 +6082,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="41" spans="1:15" ht="142.5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:15" ht="126" x14ac:dyDescent="0.35">
       <c r="A41" s="5">
         <v>39</v>
       </c>
@@ -6117,7 +6129,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="42" spans="1:15" ht="99.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:15" ht="98" hidden="1" x14ac:dyDescent="0.35">
       <c r="A42" s="5">
         <v>40</v>
       </c>
@@ -6162,7 +6174,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="43" spans="1:15" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:15" ht="42" x14ac:dyDescent="0.35">
       <c r="A43" s="5">
         <v>41</v>
       </c>
@@ -6207,7 +6219,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="44" spans="1:15" ht="71.25" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:15" ht="70" x14ac:dyDescent="0.35">
       <c r="A44" s="5">
         <v>42</v>
       </c>
@@ -6252,7 +6264,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="45" spans="1:15" ht="71.25" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:15" ht="70" x14ac:dyDescent="0.35">
       <c r="A45" s="5">
         <v>43</v>
       </c>
@@ -6297,7 +6309,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="46" spans="1:15" ht="128.25" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:15" ht="126" x14ac:dyDescent="0.35">
       <c r="A46" s="5"/>
       <c r="B46" s="6">
         <v>43427</v>
@@ -6336,7 +6348,7 @@
       <c r="N46" s="40"/>
       <c r="O46" s="42"/>
     </row>
-    <row r="47" spans="1:15" ht="57" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:15" ht="56" hidden="1" x14ac:dyDescent="0.35">
       <c r="A47" s="5"/>
       <c r="B47" s="6">
         <v>43427</v>
@@ -6375,7 +6387,7 @@
       <c r="N47" s="40"/>
       <c r="O47" s="42"/>
     </row>
-    <row r="48" spans="1:15" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:15" ht="42" x14ac:dyDescent="0.35">
       <c r="A48" s="5">
         <v>44</v>
       </c>
@@ -6422,7 +6434,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="49" spans="1:15" ht="57" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:15" ht="56" x14ac:dyDescent="0.35">
       <c r="A49" s="5">
         <v>45</v>
       </c>
@@ -6470,7 +6482,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="50" spans="1:15" ht="42.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:15" ht="42" hidden="1" x14ac:dyDescent="0.35">
       <c r="A50" s="5">
         <v>46</v>
       </c>
@@ -6514,7 +6526,7 @@
       </c>
       <c r="O50" s="42"/>
     </row>
-    <row r="51" spans="1:15" ht="156.75" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:15" ht="140" x14ac:dyDescent="0.35">
       <c r="A51" s="5">
         <v>47</v>
       </c>
@@ -6560,7 +6572,7 @@
       </c>
       <c r="O51" s="42"/>
     </row>
-    <row r="52" spans="1:15" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:15" ht="42" x14ac:dyDescent="0.35">
       <c r="A52" s="5">
         <v>48</v>
       </c>
@@ -6607,7 +6619,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="53" spans="1:15" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:15" ht="42" x14ac:dyDescent="0.35">
       <c r="A53" s="5">
         <v>49</v>
       </c>
@@ -6653,7 +6665,7 @@
       </c>
       <c r="O53" s="42"/>
     </row>
-    <row r="54" spans="1:15" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:15" ht="28" hidden="1" x14ac:dyDescent="0.35">
       <c r="A54" s="5">
         <v>50</v>
       </c>
@@ -6697,7 +6709,7 @@
       </c>
       <c r="O54" s="42"/>
     </row>
-    <row r="55" spans="1:15" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:15" ht="42" x14ac:dyDescent="0.35">
       <c r="A55" s="5">
         <v>51</v>
       </c>
@@ -6744,7 +6756,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="56" spans="1:15" ht="85.5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:15" ht="84" x14ac:dyDescent="0.35">
       <c r="A56" s="5">
         <v>52</v>
       </c>
@@ -6791,7 +6803,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="57" spans="1:15" ht="42.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:15" ht="42" hidden="1" x14ac:dyDescent="0.35">
       <c r="A57" s="5">
         <v>53</v>
       </c>
@@ -6835,7 +6847,7 @@
       </c>
       <c r="O57" s="42"/>
     </row>
-    <row r="58" spans="1:15" ht="57" hidden="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:15" ht="56" hidden="1" x14ac:dyDescent="0.35">
       <c r="A58" s="5">
         <v>54</v>
       </c>
@@ -6879,7 +6891,7 @@
       </c>
       <c r="O58" s="42"/>
     </row>
-    <row r="59" spans="1:15" ht="71.25" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:15" ht="70" x14ac:dyDescent="0.35">
       <c r="A59" s="5">
         <v>55</v>
       </c>
@@ -6924,7 +6936,7 @@
       </c>
       <c r="O59" s="42"/>
     </row>
-    <row r="60" spans="1:15" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:15" ht="42" x14ac:dyDescent="0.35">
       <c r="A60" s="5">
         <v>56</v>
       </c>
@@ -6971,7 +6983,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="61" spans="1:15" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:15" ht="42" x14ac:dyDescent="0.35">
       <c r="A61" s="5">
         <v>57</v>
       </c>
@@ -7018,7 +7030,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="62" spans="1:15" ht="99.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:15" ht="84" hidden="1" x14ac:dyDescent="0.35">
       <c r="A62" s="5">
         <v>58</v>
       </c>
@@ -7059,7 +7071,7 @@
       <c r="N62" s="43"/>
       <c r="O62" s="42"/>
     </row>
-    <row r="63" spans="1:15" ht="57" hidden="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:15" ht="56" hidden="1" x14ac:dyDescent="0.35">
       <c r="A63" s="5">
         <v>59</v>
       </c>
@@ -7100,7 +7112,7 @@
       <c r="N63" s="43"/>
       <c r="O63" s="42"/>
     </row>
-    <row r="64" spans="1:15" ht="171" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:15" ht="154" x14ac:dyDescent="0.35">
       <c r="A64" s="5">
         <v>60</v>
       </c>
@@ -7147,7 +7159,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="65" spans="1:15" ht="99.75" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:15" ht="98" x14ac:dyDescent="0.35">
       <c r="A65" s="5">
         <v>61</v>
       </c>
@@ -7187,12 +7199,14 @@
       <c r="M65" s="41">
         <v>30</v>
       </c>
-      <c r="N65" s="43"/>
+      <c r="N65" s="43">
+        <v>60</v>
+      </c>
       <c r="O65" s="42" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="66" spans="1:15" ht="99.75" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:15" ht="98" x14ac:dyDescent="0.35">
       <c r="A66" s="5">
         <v>62</v>
       </c>
@@ -7233,7 +7247,7 @@
       <c r="N66" s="43"/>
       <c r="O66" s="42"/>
     </row>
-    <row r="67" spans="1:15" ht="228" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:15" ht="210" x14ac:dyDescent="0.35">
       <c r="A67" s="5">
         <v>63</v>
       </c>
@@ -7271,10 +7285,14 @@
         <v>43446</v>
       </c>
       <c r="M67" s="41"/>
-      <c r="N67" s="5"/>
-      <c r="O67" s="42"/>
-    </row>
-    <row r="68" spans="1:15" ht="42.75" x14ac:dyDescent="0.25">
+      <c r="N67" s="43">
+        <v>24</v>
+      </c>
+      <c r="O67" s="42" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="68" spans="1:15" ht="42" x14ac:dyDescent="0.35">
       <c r="A68" s="5">
         <v>64</v>
       </c>
@@ -7312,10 +7330,12 @@
         <v>43446</v>
       </c>
       <c r="M68" s="41"/>
-      <c r="N68" s="5"/>
+      <c r="N68" s="43">
+        <v>4</v>
+      </c>
       <c r="O68" s="42"/>
     </row>
-    <row r="69" spans="1:15" ht="106.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:15" ht="106.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A69" s="5">
         <v>65</v>
       </c>
@@ -7353,10 +7373,14 @@
         <v>43451</v>
       </c>
       <c r="M69" s="41"/>
-      <c r="N69" s="5"/>
-      <c r="O69" s="42"/>
-    </row>
-    <row r="70" spans="1:15" ht="57" x14ac:dyDescent="0.25">
+      <c r="N69" s="43">
+        <v>18</v>
+      </c>
+      <c r="O69" s="42" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="70" spans="1:15" ht="42" x14ac:dyDescent="0.35">
       <c r="A70" s="5">
         <v>66</v>
       </c>
@@ -7394,11 +7418,13 @@
         <v>43452</v>
       </c>
       <c r="M70" s="41"/>
-      <c r="N70" s="5"/>
+      <c r="N70" s="43">
+        <v>16</v>
+      </c>
       <c r="O70" s="42"/>
     </row>
   </sheetData>
-  <autoFilter ref="A2:O70" xr:uid="{00000000-0009-0000-0000-000000000000}">
+  <autoFilter ref="A2:O70">
     <filterColumn colId="8">
       <filters>
         <filter val="1"/>
@@ -7415,57 +7441,57 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="34.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B3" s="17" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B4" s="7" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="5" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B5" s="7" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B6" s="7" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="7" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B7" s="7" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="8" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B8" s="13" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="9" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B9" s="13" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="10" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B10" s="13" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="11" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B11" s="13"/>
     </row>
   </sheetData>
@@ -7475,19 +7501,19 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2566BF77-9AEC-4C43-B6A9-D1A01F909B3F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="34.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="34.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="44" t="s">
         <v>195</v>
       </c>
@@ -7498,7 +7524,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="45" t="s">
         <v>91</v>
       </c>
@@ -7509,7 +7535,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="45" t="s">
         <v>39</v>
       </c>
@@ -7520,7 +7546,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" s="45" t="s">
         <v>163</v>
       </c>
@@ -7531,7 +7557,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="45" t="s">
         <v>99</v>
       </c>
@@ -7542,7 +7568,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" s="45" t="s">
         <v>16</v>
       </c>
@@ -7553,7 +7579,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" s="45" t="s">
         <v>48</v>
       </c>
@@ -7564,7 +7590,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" s="45" t="s">
         <v>68</v>
       </c>
@@ -7575,7 +7601,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" s="45" t="s">
         <v>196</v>
       </c>
@@ -7616,6 +7642,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D32E068FDE16E34B8075022FB1536456" ma:contentTypeVersion="5" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d905b7d076fda08b8ad7ac1f301e6870">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7784986bdb25cf89cb05135ef15ccb6c" ns1:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -7787,15 +7822,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0212785F-078B-445B-9297-945E33C92ACD}">
   <ds:schemaRefs>
@@ -7813,6 +7839,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6B8E61E4-4805-4EED-8CD4-7E0EB2F2E46E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62A013D4-4E69-4E0D-8B8F-1AA53B7A2CEA}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -7828,12 +7862,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6B8E61E4-4805-4EED-8CD4-7E0EB2F2E46E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
added estimates for IDA CR
</commit_message>
<xml_diff>
--- a/requirements/MOSIP_Requirements Change_Tracker_18Dec18_Updated.xlsx
+++ b/requirements/MOSIP_Requirements Change_Tracker_18Dec18_Updated.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MOSIP_GIT_HUB\requirements\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Mindtree\Projects\MOSIP\IDA\Code\git-repo\master-branch\mosip\requirements\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -21,7 +21,7 @@
   </definedNames>
   <calcPr calcId="162913"/>
   <pivotCaches>
-    <pivotCache cacheId="1" r:id="rId4"/>
+    <pivotCache cacheId="5" r:id="rId4"/>
   </pivotCaches>
   <fileRecoveryPr autoRecover="0"/>
   <extLst>
@@ -1325,9 +1325,6 @@
 Phonetics match should be considered as part of v2</t>
   </si>
   <si>
-    <t>Considering only exact match for Demo Auth, both partial and phonetics are to be disabled - needs to be made configurable at country level and validation for this needs to be added</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <u/>
@@ -1355,9 +1352,6 @@
   </si>
   <si>
     <t>As concluded with Sanjay, MOSIP should consider only exact match strategy</t>
-  </si>
-  <si>
-    <t>Will be taken care as part of S.No. 31</t>
   </si>
   <si>
     <r>
@@ -2022,9 +2016,6 @@
     <t>Query log review with Anadi/Ramesh (JIRA) on 06-Dec-18</t>
   </si>
   <si>
-    <t>Assuming that we will have multiple license keys per TSP, which will be then mapped to multiple allowed Auth types and a separate functionality to generate Licence Keys would be required in Admin Portal</t>
-  </si>
-  <si>
     <t>GoM Requirements</t>
   </si>
   <si>
@@ -2340,6 +2331,16 @@
     <t xml:space="preserve">1. Pre-Reg Sync/Batch Job Changes
 2. Multi-lingual changes 
 3. ID object based strucutre changes </t>
+  </si>
+  <si>
+    <t>Considering only exact match for Demo Auth, both partial and phonetics are to be disabled and only validations and configurations for exact match will be added</t>
+  </si>
+  <si>
+    <t>Will be taken care as part of S.No. 33</t>
+  </si>
+  <si>
+    <t>Assuming that we will have multiple license keys per TSP, which will be then mapped to multiple allowed Auth types, we will have to build generate and validate functionalities for license keys and mapping them as above.
+Separate UI to generate Licence Keys, map them to a TSP and then map auth types to a license key would be required in Admin Portal, which is not factored in this estimates.</t>
   </si>
 </sst>
 </file>
@@ -3895,7 +3896,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:C11" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="15">
     <pivotField dataField="1" showAll="0"/>
@@ -4247,9 +4248,9 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:O70"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A68" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D70" sqref="D70"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="N64" sqref="N64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.26953125" defaultRowHeight="14" x14ac:dyDescent="0.35"/>
@@ -4329,7 +4330,7 @@
         <v>12</v>
       </c>
       <c r="M2" s="34" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="N2" s="34" t="s">
         <v>13</v>
@@ -4338,7 +4339,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:15" s="4" customFormat="1" ht="112" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:15" s="4" customFormat="1" ht="112" hidden="1" x14ac:dyDescent="0.35">
       <c r="A3" s="5">
         <v>1</v>
       </c>
@@ -4379,13 +4380,13 @@
         <v>36</v>
       </c>
       <c r="N3" s="40" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="O3" s="28" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:15" s="4" customFormat="1" ht="56" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:15" s="4" customFormat="1" ht="56" hidden="1" x14ac:dyDescent="0.35">
       <c r="A4" s="5">
         <v>2</v>
       </c>
@@ -4432,7 +4433,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:15" s="4" customFormat="1" ht="70" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:15" s="4" customFormat="1" ht="70" hidden="1" x14ac:dyDescent="0.35">
       <c r="A5" s="5">
         <v>3</v>
       </c>
@@ -4473,13 +4474,13 @@
         <v>35</v>
       </c>
       <c r="N5" s="40" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="O5" s="28" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:15" s="4" customFormat="1" ht="56" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:15" s="4" customFormat="1" ht="56" hidden="1" x14ac:dyDescent="0.35">
       <c r="A6" s="5">
         <v>4</v>
       </c>
@@ -4520,13 +4521,13 @@
         <v>30</v>
       </c>
       <c r="N6" s="40" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="O6" s="29" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:15" s="1" customFormat="1" ht="42" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:15" s="1" customFormat="1" ht="42" hidden="1" x14ac:dyDescent="0.3">
       <c r="A7" s="5">
         <v>5</v>
       </c>
@@ -4572,7 +4573,7 @@
       </c>
       <c r="O7" s="28"/>
     </row>
-    <row r="8" spans="1:15" s="1" customFormat="1" ht="56" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:15" s="1" customFormat="1" ht="56" hidden="1" x14ac:dyDescent="0.3">
       <c r="A8" s="5">
         <v>6</v>
       </c>
@@ -4613,7 +4614,7 @@
         <v>36</v>
       </c>
       <c r="N8" s="40" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="O8" s="28"/>
     </row>
@@ -4661,7 +4662,7 @@
       </c>
       <c r="O9" s="28"/>
     </row>
-    <row r="10" spans="1:15" s="1" customFormat="1" ht="56" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:15" s="1" customFormat="1" ht="56" hidden="1" x14ac:dyDescent="0.3">
       <c r="A10" s="5">
         <v>8</v>
       </c>
@@ -4702,13 +4703,13 @@
         <v>20</v>
       </c>
       <c r="N10" s="40" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="O10" s="28" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="11" spans="1:15" s="1" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:15" s="1" customFormat="1" ht="75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="5">
         <v>9</v>
       </c>
@@ -4755,7 +4756,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="12" spans="1:15" s="1" customFormat="1" ht="112" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:15" s="1" customFormat="1" ht="112" hidden="1" x14ac:dyDescent="0.3">
       <c r="A12" s="5">
         <v>10</v>
       </c>
@@ -4796,13 +4797,13 @@
         <v>55</v>
       </c>
       <c r="N12" s="40" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="O12" s="28" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="13" spans="1:15" s="4" customFormat="1" ht="154" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:15" s="4" customFormat="1" ht="154" hidden="1" x14ac:dyDescent="0.35">
       <c r="A13" s="5">
         <v>11</v>
       </c>
@@ -4843,13 +4844,13 @@
         <v>59</v>
       </c>
       <c r="N13" s="40" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="O13" s="28" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="14" spans="1:15" s="1" customFormat="1" ht="98" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:15" s="1" customFormat="1" ht="98" hidden="1" x14ac:dyDescent="0.3">
       <c r="A14" s="5">
         <v>12</v>
       </c>
@@ -4890,11 +4891,11 @@
         <v>63</v>
       </c>
       <c r="N14" s="40" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="O14" s="28"/>
     </row>
-    <row r="15" spans="1:15" s="4" customFormat="1" ht="98" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:15" s="4" customFormat="1" ht="98" hidden="1" x14ac:dyDescent="0.35">
       <c r="A15" s="5">
         <v>13</v>
       </c>
@@ -4935,13 +4936,13 @@
         <v>66</v>
       </c>
       <c r="N15" s="40" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="O15" s="28" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="16" spans="1:15" s="1" customFormat="1" ht="42" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:15" s="1" customFormat="1" ht="42" hidden="1" x14ac:dyDescent="0.3">
       <c r="A16" s="5">
         <v>14</v>
       </c>
@@ -4977,7 +4978,7 @@
         <v>43419</v>
       </c>
       <c r="M16" s="40" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="N16" s="40">
         <f t="shared" si="0"/>
@@ -4985,7 +4986,7 @@
       </c>
       <c r="O16" s="28"/>
     </row>
-    <row r="17" spans="1:15" s="4" customFormat="1" ht="42" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:15" s="4" customFormat="1" ht="42" hidden="1" x14ac:dyDescent="0.35">
       <c r="A17" s="5">
         <v>15</v>
       </c>
@@ -5021,7 +5022,7 @@
         <v>43419</v>
       </c>
       <c r="M17" s="40" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="N17" s="40">
         <f t="shared" si="0"/>
@@ -5029,7 +5030,7 @@
       </c>
       <c r="O17" s="28"/>
     </row>
-    <row r="18" spans="1:15" ht="84" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:15" ht="84" hidden="1" x14ac:dyDescent="0.35">
       <c r="A18" s="5">
         <v>16</v>
       </c>
@@ -5076,7 +5077,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="19" spans="1:15" ht="84" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:15" ht="84" hidden="1" x14ac:dyDescent="0.35">
       <c r="A19" s="5">
         <v>17</v>
       </c>
@@ -5117,13 +5118,13 @@
         <v>5</v>
       </c>
       <c r="N19" s="40" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="O19" s="28" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="20" spans="1:15" ht="84" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:15" ht="84" hidden="1" x14ac:dyDescent="0.35">
       <c r="A20" s="5">
         <v>18</v>
       </c>
@@ -5164,13 +5165,13 @@
         <v>79</v>
       </c>
       <c r="N20" s="40" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="O20" s="28" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="21" spans="1:15" ht="84" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:15" ht="84" hidden="1" x14ac:dyDescent="0.35">
       <c r="A21" s="5">
         <v>19</v>
       </c>
@@ -5208,14 +5209,14 @@
         <v>43419</v>
       </c>
       <c r="M21" s="40" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="N21" s="40" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="O21" s="28"/>
     </row>
-    <row r="22" spans="1:15" ht="84" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:15" ht="84" hidden="1" x14ac:dyDescent="0.35">
       <c r="A22" s="5">
         <v>20</v>
       </c>
@@ -5253,14 +5254,14 @@
         <v>43419</v>
       </c>
       <c r="M22" s="40" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="N22" s="40" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="O22" s="28"/>
     </row>
-    <row r="23" spans="1:15" ht="84" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:15" ht="84" hidden="1" x14ac:dyDescent="0.35">
       <c r="A23" s="5">
         <v>21</v>
       </c>
@@ -5307,7 +5308,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="24" spans="1:15" ht="84" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:15" ht="84" hidden="1" x14ac:dyDescent="0.35">
       <c r="A24" s="5">
         <v>22</v>
       </c>
@@ -5348,13 +5349,13 @@
         <v>5</v>
       </c>
       <c r="N24" s="40" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="O24" s="30" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="25" spans="1:15" ht="84" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:15" ht="84" hidden="1" x14ac:dyDescent="0.35">
       <c r="A25" s="5">
         <v>23</v>
       </c>
@@ -5395,11 +5396,11 @@
         <v>0</v>
       </c>
       <c r="N25" s="40" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="O25" s="28"/>
     </row>
-    <row r="26" spans="1:15" ht="42" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:15" ht="42" hidden="1" x14ac:dyDescent="0.35">
       <c r="A26" s="5">
         <v>24</v>
       </c>
@@ -5440,11 +5441,11 @@
         <v>30</v>
       </c>
       <c r="N26" s="40" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="O26" s="20"/>
     </row>
-    <row r="27" spans="1:15" ht="70" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:15" ht="70" hidden="1" x14ac:dyDescent="0.35">
       <c r="A27" s="5">
         <v>25</v>
       </c>
@@ -5491,7 +5492,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="28" spans="1:15" ht="42" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:15" ht="42" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="5">
         <v>26</v>
       </c>
@@ -5508,7 +5509,7 @@
         <v>32</v>
       </c>
       <c r="F28" s="42" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="G28" s="20" t="s">
         <v>46</v>
@@ -5529,7 +5530,7 @@
       </c>
       <c r="O28" s="42"/>
     </row>
-    <row r="29" spans="1:15" s="11" customFormat="1" ht="84" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:15" s="11" customFormat="1" ht="84" hidden="1" x14ac:dyDescent="0.35">
       <c r="A29" s="5">
         <v>27</v>
       </c>
@@ -5576,7 +5577,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="30" spans="1:15" s="11" customFormat="1" ht="42" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:15" s="11" customFormat="1" ht="42" hidden="1" x14ac:dyDescent="0.35">
       <c r="A30" s="5">
         <v>28</v>
       </c>
@@ -5623,7 +5624,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="31" spans="1:15" ht="42" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:15" ht="42" hidden="1" x14ac:dyDescent="0.35">
       <c r="A31" s="5">
         <v>29</v>
       </c>
@@ -5664,7 +5665,7 @@
         <v>1</v>
       </c>
       <c r="N31" s="40" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="O31" s="20"/>
     </row>
@@ -5760,7 +5761,7 @@
         <v>79</v>
       </c>
       <c r="O33" s="42" t="s">
-        <v>115</v>
+        <v>213</v>
       </c>
     </row>
     <row r="34" spans="1:15" ht="140" x14ac:dyDescent="0.35">
@@ -5780,13 +5781,13 @@
         <v>32</v>
       </c>
       <c r="F34" s="10" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G34" s="20" t="s">
         <v>46</v>
       </c>
       <c r="H34" s="42" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="I34" s="42">
         <v>1</v>
@@ -5808,7 +5809,7 @@
         <v>0</v>
       </c>
       <c r="O34" s="42" t="s">
-        <v>118</v>
+        <v>214</v>
       </c>
     </row>
     <row r="35" spans="1:15" ht="70" x14ac:dyDescent="0.35">
@@ -5828,13 +5829,13 @@
         <v>32</v>
       </c>
       <c r="F35" s="10" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="G35" s="20" t="s">
         <v>46</v>
       </c>
       <c r="H35" s="42" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="I35" s="42">
         <v>1</v>
@@ -5856,7 +5857,7 @@
         <v>0</v>
       </c>
       <c r="O35" s="42" t="s">
-        <v>118</v>
+        <v>214</v>
       </c>
     </row>
     <row r="36" spans="1:15" ht="36" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
@@ -5867,7 +5868,7 @@
         <v>43430</v>
       </c>
       <c r="C36" s="20" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D36" s="42" t="s">
         <v>99</v>
@@ -5876,13 +5877,13 @@
         <v>40</v>
       </c>
       <c r="F36" s="42" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="G36" s="20" t="s">
         <v>46</v>
       </c>
       <c r="H36" s="42" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="I36" s="42">
         <v>2</v>
@@ -5911,7 +5912,7 @@
         <v>43430</v>
       </c>
       <c r="C37" s="20" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D37" s="42" t="s">
         <v>16</v>
@@ -5920,13 +5921,13 @@
         <v>40</v>
       </c>
       <c r="F37" s="42" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="G37" s="20" t="s">
         <v>46</v>
       </c>
       <c r="H37" s="42" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="I37" s="42">
         <v>2</v>
@@ -5955,7 +5956,7 @@
         <v>43427</v>
       </c>
       <c r="C38" s="20" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D38" s="42" t="s">
         <v>16</v>
@@ -5964,16 +5965,16 @@
         <v>40</v>
       </c>
       <c r="F38" s="42" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="G38" s="20" t="s">
         <v>46</v>
       </c>
       <c r="H38" s="42" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="I38" s="42" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="J38" s="42" t="s">
         <v>93</v>
@@ -5999,7 +6000,7 @@
         <v>43427</v>
       </c>
       <c r="C39" s="20" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D39" s="42" t="s">
         <v>16</v>
@@ -6008,7 +6009,7 @@
         <v>40</v>
       </c>
       <c r="F39" s="42" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="G39" s="20" t="s">
         <v>46</v>
@@ -6035,7 +6036,7 @@
       </c>
       <c r="O39" s="42"/>
     </row>
-    <row r="40" spans="1:15" ht="252" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:15" ht="252" hidden="1" x14ac:dyDescent="0.35">
       <c r="A40" s="5">
         <v>38</v>
       </c>
@@ -6043,7 +6044,7 @@
         <v>43427</v>
       </c>
       <c r="C40" s="20" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D40" s="42" t="s">
         <v>48</v>
@@ -6052,16 +6053,16 @@
         <v>32</v>
       </c>
       <c r="F40" s="42" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="G40" s="20" t="s">
         <v>46</v>
       </c>
       <c r="H40" s="42" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="I40" s="42" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="J40" s="42" t="s">
         <v>93</v>
@@ -6073,16 +6074,16 @@
         <v>43440</v>
       </c>
       <c r="M40" s="40" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="N40" s="40" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="O40" s="42" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="41" spans="1:15" ht="126" x14ac:dyDescent="0.35">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15" ht="126" hidden="1" x14ac:dyDescent="0.35">
       <c r="A41" s="5">
         <v>39</v>
       </c>
@@ -6090,7 +6091,7 @@
         <v>43427</v>
       </c>
       <c r="C41" s="20" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D41" s="42" t="s">
         <v>48</v>
@@ -6099,13 +6100,13 @@
         <v>32</v>
       </c>
       <c r="F41" s="42" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="G41" s="20" t="s">
         <v>46</v>
       </c>
       <c r="H41" s="42" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="I41" s="42">
         <v>1</v>
@@ -6120,10 +6121,10 @@
         <v>43440</v>
       </c>
       <c r="M41" s="40" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="N41" s="40" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="O41" s="42" t="s">
         <v>60</v>
@@ -6137,7 +6138,7 @@
         <v>43427</v>
       </c>
       <c r="C42" s="20" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D42" s="42" t="s">
         <v>48</v>
@@ -6146,13 +6147,13 @@
         <v>40</v>
       </c>
       <c r="F42" s="42" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="G42" s="20" t="s">
         <v>46</v>
       </c>
       <c r="H42" s="42" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="I42" s="42">
         <v>2</v>
@@ -6171,10 +6172,10 @@
       </c>
       <c r="N42" s="40"/>
       <c r="O42" s="42" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="43" spans="1:15" ht="42" x14ac:dyDescent="0.35">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15" ht="42" hidden="1" x14ac:dyDescent="0.35">
       <c r="A43" s="5">
         <v>41</v>
       </c>
@@ -6182,7 +6183,7 @@
         <v>43427</v>
       </c>
       <c r="C43" s="20" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D43" s="42" t="s">
         <v>48</v>
@@ -6191,13 +6192,13 @@
         <v>32</v>
       </c>
       <c r="F43" s="42" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="G43" s="20" t="s">
         <v>46</v>
       </c>
       <c r="H43" s="42" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="I43" s="42">
         <v>1</v>
@@ -6216,10 +6217,10 @@
       </c>
       <c r="N43" s="40"/>
       <c r="O43" s="42" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="44" spans="1:15" ht="70" x14ac:dyDescent="0.35">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15" ht="70" hidden="1" x14ac:dyDescent="0.35">
       <c r="A44" s="5">
         <v>42</v>
       </c>
@@ -6227,7 +6228,7 @@
         <v>43427</v>
       </c>
       <c r="C44" s="20" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D44" s="42" t="s">
         <v>48</v>
@@ -6236,7 +6237,7 @@
         <v>32</v>
       </c>
       <c r="F44" s="42" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="G44" s="20" t="s">
         <v>46</v>
@@ -6261,10 +6262,10 @@
       </c>
       <c r="N44" s="40"/>
       <c r="O44" s="42" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="45" spans="1:15" ht="70" x14ac:dyDescent="0.35">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15" ht="70" hidden="1" x14ac:dyDescent="0.35">
       <c r="A45" s="5">
         <v>43</v>
       </c>
@@ -6272,7 +6273,7 @@
         <v>43427</v>
       </c>
       <c r="C45" s="20" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D45" s="42" t="s">
         <v>48</v>
@@ -6281,13 +6282,13 @@
         <v>32</v>
       </c>
       <c r="F45" s="42" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="G45" s="20" t="s">
         <v>46</v>
       </c>
       <c r="H45" s="42" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="I45" s="42">
         <v>1</v>
@@ -6296,7 +6297,7 @@
         <v>93</v>
       </c>
       <c r="K45" s="42" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="L45" s="28">
         <v>43452</v>
@@ -6306,16 +6307,16 @@
       </c>
       <c r="N45" s="40"/>
       <c r="O45" s="42" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="46" spans="1:15" ht="126" x14ac:dyDescent="0.35">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15" ht="126" hidden="1" x14ac:dyDescent="0.35">
       <c r="A46" s="5"/>
       <c r="B46" s="6">
         <v>43427</v>
       </c>
       <c r="C46" s="20" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D46" s="42" t="s">
         <v>48</v>
@@ -6324,22 +6325,22 @@
         <v>32</v>
       </c>
       <c r="F46" s="42" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="G46" s="20" t="s">
         <v>46</v>
       </c>
       <c r="H46" s="42" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="I46" s="42" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="J46" s="42" t="s">
         <v>93</v>
       </c>
       <c r="K46" s="42" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="L46" s="28">
         <v>43452</v>
@@ -6354,7 +6355,7 @@
         <v>43427</v>
       </c>
       <c r="C47" s="20" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D47" s="42" t="s">
         <v>48</v>
@@ -6363,13 +6364,13 @@
         <v>32</v>
       </c>
       <c r="F47" s="42" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="G47" s="20" t="s">
         <v>46</v>
       </c>
       <c r="H47" s="42" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="I47" s="42">
         <v>2</v>
@@ -6378,7 +6379,7 @@
         <v>93</v>
       </c>
       <c r="K47" s="42" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="L47" s="28">
         <v>43452</v>
@@ -6387,7 +6388,7 @@
       <c r="N47" s="40"/>
       <c r="O47" s="42"/>
     </row>
-    <row r="48" spans="1:15" ht="42" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:15" ht="42" hidden="1" x14ac:dyDescent="0.35">
       <c r="A48" s="5">
         <v>44</v>
       </c>
@@ -6395,7 +6396,7 @@
         <v>43427</v>
       </c>
       <c r="C48" s="20" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D48" s="42" t="s">
         <v>48</v>
@@ -6404,7 +6405,7 @@
         <v>32</v>
       </c>
       <c r="F48" s="42" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="G48" s="20" t="s">
         <v>46</v>
@@ -6425,13 +6426,13 @@
         <v>43440</v>
       </c>
       <c r="M48" s="40" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="N48" s="40" t="s">
         <v>51</v>
       </c>
       <c r="O48" s="42" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="49" spans="1:15" ht="56" x14ac:dyDescent="0.35">
@@ -6442,7 +6443,7 @@
         <v>43427</v>
       </c>
       <c r="C49" s="20" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D49" s="42" t="s">
         <v>39</v>
@@ -6451,13 +6452,13 @@
         <v>32</v>
       </c>
       <c r="F49" s="42" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="G49" s="20" t="s">
         <v>46</v>
       </c>
       <c r="H49" s="26" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="I49" s="42">
         <v>1</v>
@@ -6479,7 +6480,7 @@
         <v>0</v>
       </c>
       <c r="O49" s="42" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="50" spans="1:15" ht="42" hidden="1" x14ac:dyDescent="0.35">
@@ -6490,7 +6491,7 @@
         <v>43427</v>
       </c>
       <c r="C50" s="20" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D50" s="42" t="s">
         <v>16</v>
@@ -6499,13 +6500,13 @@
         <v>40</v>
       </c>
       <c r="F50" s="42" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="G50" s="20" t="s">
         <v>46</v>
       </c>
       <c r="H50" s="42" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="I50" s="42">
         <v>2</v>
@@ -6526,7 +6527,7 @@
       </c>
       <c r="O50" s="42"/>
     </row>
-    <row r="51" spans="1:15" ht="140" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:15" ht="140" hidden="1" x14ac:dyDescent="0.35">
       <c r="A51" s="5">
         <v>47</v>
       </c>
@@ -6534,7 +6535,7 @@
         <v>43427</v>
       </c>
       <c r="C51" s="20" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D51" s="42" t="s">
         <v>68</v>
@@ -6543,13 +6544,13 @@
         <v>32</v>
       </c>
       <c r="F51" s="42" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="G51" s="20" t="s">
         <v>46</v>
       </c>
       <c r="H51" s="42" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="I51" s="42">
         <v>1</v>
@@ -6572,7 +6573,7 @@
       </c>
       <c r="O51" s="42"/>
     </row>
-    <row r="52" spans="1:15" ht="42" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:15" ht="42" hidden="1" x14ac:dyDescent="0.35">
       <c r="A52" s="5">
         <v>48</v>
       </c>
@@ -6580,7 +6581,7 @@
         <v>43427</v>
       </c>
       <c r="C52" s="20" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D52" s="42" t="s">
         <v>16</v>
@@ -6589,7 +6590,7 @@
         <v>32</v>
       </c>
       <c r="F52" s="42" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="G52" s="20" t="s">
         <v>46</v>
@@ -6616,10 +6617,10 @@
         <v>51</v>
       </c>
       <c r="O52" s="42" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="53" spans="1:15" ht="42" x14ac:dyDescent="0.35">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="53" spans="1:15" ht="42" hidden="1" x14ac:dyDescent="0.35">
       <c r="A53" s="5">
         <v>49</v>
       </c>
@@ -6627,7 +6628,7 @@
         <v>43427</v>
       </c>
       <c r="C53" s="20" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D53" s="42" t="s">
         <v>68</v>
@@ -6636,7 +6637,7 @@
         <v>32</v>
       </c>
       <c r="F53" s="42" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G53" s="20" t="s">
         <v>46</v>
@@ -6673,7 +6674,7 @@
         <v>43427</v>
       </c>
       <c r="C54" s="20" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D54" s="42" t="s">
         <v>16</v>
@@ -6682,13 +6683,13 @@
         <v>40</v>
       </c>
       <c r="F54" s="42" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="G54" s="20" t="s">
         <v>46</v>
       </c>
       <c r="H54" s="42" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="I54" s="42">
         <v>2</v>
@@ -6709,7 +6710,7 @@
       </c>
       <c r="O54" s="42"/>
     </row>
-    <row r="55" spans="1:15" ht="42" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:15" ht="42" hidden="1" x14ac:dyDescent="0.35">
       <c r="A55" s="5">
         <v>51</v>
       </c>
@@ -6717,7 +6718,7 @@
         <v>43427</v>
       </c>
       <c r="C55" s="20" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D55" s="42" t="s">
         <v>16</v>
@@ -6726,7 +6727,7 @@
         <v>32</v>
       </c>
       <c r="F55" s="42" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="G55" s="20" t="s">
         <v>46</v>
@@ -6750,13 +6751,13 @@
         <v>20</v>
       </c>
       <c r="N55" s="40" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="O55" s="42" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="56" spans="1:15" ht="84" x14ac:dyDescent="0.35">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="56" spans="1:15" ht="84" hidden="1" x14ac:dyDescent="0.35">
       <c r="A56" s="5">
         <v>52</v>
       </c>
@@ -6764,7 +6765,7 @@
         <v>43427</v>
       </c>
       <c r="C56" s="20" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D56" s="42" t="s">
         <v>16</v>
@@ -6773,13 +6774,13 @@
         <v>32</v>
       </c>
       <c r="F56" s="42" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="G56" s="20" t="s">
         <v>46</v>
       </c>
       <c r="H56" s="42" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="I56" s="42">
         <v>1</v>
@@ -6797,10 +6798,10 @@
         <v>40</v>
       </c>
       <c r="N56" s="40" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="O56" s="42" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="57" spans="1:15" ht="42" hidden="1" x14ac:dyDescent="0.35">
@@ -6811,7 +6812,7 @@
         <v>43427</v>
       </c>
       <c r="C57" s="20" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D57" s="42" t="s">
         <v>16</v>
@@ -6820,13 +6821,13 @@
         <v>40</v>
       </c>
       <c r="F57" s="42" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="G57" s="20" t="s">
         <v>46</v>
       </c>
       <c r="H57" s="42" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="I57" s="42">
         <v>2</v>
@@ -6855,7 +6856,7 @@
         <v>43427</v>
       </c>
       <c r="C58" s="20" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D58" s="42" t="s">
         <v>16</v>
@@ -6864,13 +6865,13 @@
         <v>40</v>
       </c>
       <c r="F58" s="42" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="G58" s="20" t="s">
         <v>46</v>
       </c>
       <c r="H58" s="42" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="I58" s="42">
         <v>2</v>
@@ -6891,7 +6892,7 @@
       </c>
       <c r="O58" s="42"/>
     </row>
-    <row r="59" spans="1:15" ht="70" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:15" ht="70" hidden="1" x14ac:dyDescent="0.35">
       <c r="A59" s="5">
         <v>55</v>
       </c>
@@ -6899,16 +6900,16 @@
         <v>43432</v>
       </c>
       <c r="C59" s="42" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="D59" s="42" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="E59" s="42" t="s">
         <v>32</v>
       </c>
       <c r="F59" s="42" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="G59" s="20" t="s">
         <v>46</v>
@@ -6932,7 +6933,7 @@
         <v>4</v>
       </c>
       <c r="N59" s="40" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="O59" s="42"/>
     </row>
@@ -6944,7 +6945,7 @@
         <v>43432</v>
       </c>
       <c r="C60" s="20" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D60" s="42" t="s">
         <v>39</v>
@@ -6953,7 +6954,7 @@
         <v>32</v>
       </c>
       <c r="F60" s="42" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="G60" s="20" t="s">
         <v>46</v>
@@ -6980,10 +6981,10 @@
         <v>0</v>
       </c>
       <c r="O60" s="42" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="61" spans="1:15" ht="42" x14ac:dyDescent="0.35">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="61" spans="1:15" ht="42" hidden="1" x14ac:dyDescent="0.35">
       <c r="A61" s="5">
         <v>57</v>
       </c>
@@ -6991,7 +6992,7 @@
         <v>43432</v>
       </c>
       <c r="C61" s="20" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D61" s="42" t="s">
         <v>48</v>
@@ -7000,7 +7001,7 @@
         <v>32</v>
       </c>
       <c r="F61" s="42" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="G61" s="20" t="s">
         <v>46</v>
@@ -7027,7 +7028,7 @@
         <v>66</v>
       </c>
       <c r="O61" s="42" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="62" spans="1:15" ht="84" hidden="1" x14ac:dyDescent="0.35">
@@ -7038,22 +7039,22 @@
         <v>43432</v>
       </c>
       <c r="C62" s="42" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="D62" s="42" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="E62" s="42" t="s">
         <v>40</v>
       </c>
       <c r="F62" s="42" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="G62" s="20" t="s">
         <v>46</v>
       </c>
       <c r="H62" s="42" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="I62" s="42">
         <v>2</v>
@@ -7079,25 +7080,25 @@
         <v>43432</v>
       </c>
       <c r="C63" s="42" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="D63" s="42" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="E63" s="42" t="s">
         <v>40</v>
       </c>
       <c r="F63" s="42" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="G63" s="20" t="s">
         <v>46</v>
       </c>
       <c r="H63" s="42" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="I63" s="42" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="J63" s="42" t="s">
         <v>93</v>
@@ -7120,7 +7121,7 @@
         <v>43440</v>
       </c>
       <c r="C64" s="42" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D64" s="42" t="s">
         <v>39</v>
@@ -7129,7 +7130,7 @@
         <v>32</v>
       </c>
       <c r="F64" s="42" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="G64" s="20" t="s">
         <v>46</v>
@@ -7144,7 +7145,7 @@
         <v>93</v>
       </c>
       <c r="K64" s="42" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="L64" s="28">
         <v>43452</v>
@@ -7153,13 +7154,13 @@
         <v>15</v>
       </c>
       <c r="N64" s="5">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="O64" s="42" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="65" spans="1:15" ht="98" x14ac:dyDescent="0.35">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="65" spans="1:15" ht="98" hidden="1" x14ac:dyDescent="0.35">
       <c r="A65" s="5">
         <v>61</v>
       </c>
@@ -7167,7 +7168,7 @@
         <v>43440</v>
       </c>
       <c r="C65" s="20" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="D65" s="42" t="s">
         <v>16</v>
@@ -7176,7 +7177,7 @@
         <v>32</v>
       </c>
       <c r="F65" s="42" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="G65" s="20" t="s">
         <v>46</v>
@@ -7185,7 +7186,7 @@
         <v>105</v>
       </c>
       <c r="I65" s="42" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="J65" s="42" t="s">
         <v>93</v>
@@ -7203,10 +7204,10 @@
         <v>60</v>
       </c>
       <c r="O65" s="42" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="66" spans="1:15" ht="98" x14ac:dyDescent="0.35">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="66" spans="1:15" ht="98" hidden="1" x14ac:dyDescent="0.35">
       <c r="A66" s="5">
         <v>62</v>
       </c>
@@ -7214,7 +7215,7 @@
         <v>43440</v>
       </c>
       <c r="C66" s="20" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="D66" s="42" t="s">
         <v>99</v>
@@ -7223,7 +7224,7 @@
         <v>32</v>
       </c>
       <c r="F66" s="42" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="G66" s="20" t="s">
         <v>46</v>
@@ -7232,7 +7233,7 @@
         <v>105</v>
       </c>
       <c r="I66" s="42" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="J66" s="42" t="s">
         <v>93</v>
@@ -7247,7 +7248,7 @@
       <c r="N66" s="43"/>
       <c r="O66" s="42"/>
     </row>
-    <row r="67" spans="1:15" ht="210" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:15" ht="210" hidden="1" x14ac:dyDescent="0.35">
       <c r="A67" s="5">
         <v>63</v>
       </c>
@@ -7255,7 +7256,7 @@
         <v>43446</v>
       </c>
       <c r="C67" s="42" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="D67" s="42" t="s">
         <v>16</v>
@@ -7264,7 +7265,7 @@
         <v>32</v>
       </c>
       <c r="F67" s="42" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="G67" s="20" t="s">
         <v>46</v>
@@ -7289,10 +7290,10 @@
         <v>24</v>
       </c>
       <c r="O67" s="42" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="68" spans="1:15" ht="42" x14ac:dyDescent="0.35">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="68" spans="1:15" ht="42" hidden="1" x14ac:dyDescent="0.35">
       <c r="A68" s="5">
         <v>64</v>
       </c>
@@ -7300,7 +7301,7 @@
         <v>43446</v>
       </c>
       <c r="C68" s="42" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="D68" s="42" t="s">
         <v>16</v>
@@ -7309,7 +7310,7 @@
         <v>32</v>
       </c>
       <c r="F68" s="42" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="G68" s="20" t="s">
         <v>46</v>
@@ -7335,7 +7336,7 @@
       </c>
       <c r="O68" s="42"/>
     </row>
-    <row r="69" spans="1:15" ht="106.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:15" ht="106.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A69" s="5">
         <v>65</v>
       </c>
@@ -7343,7 +7344,7 @@
         <v>43451</v>
       </c>
       <c r="C69" s="42" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="D69" s="42" t="s">
         <v>16</v>
@@ -7352,7 +7353,7 @@
         <v>32</v>
       </c>
       <c r="F69" s="42" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="G69" s="20" t="s">
         <v>46</v>
@@ -7377,10 +7378,10 @@
         <v>18</v>
       </c>
       <c r="O69" s="42" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="70" spans="1:15" ht="42" x14ac:dyDescent="0.35">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="70" spans="1:15" ht="42" hidden="1" x14ac:dyDescent="0.35">
       <c r="A70" s="5">
         <v>66</v>
       </c>
@@ -7388,7 +7389,7 @@
         <v>43451</v>
       </c>
       <c r="C70" s="42" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="D70" s="42" t="s">
         <v>16</v>
@@ -7397,7 +7398,7 @@
         <v>32</v>
       </c>
       <c r="F70" s="42" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="G70" s="20" t="s">
         <v>46</v>
@@ -7425,6 +7426,11 @@
     </row>
   </sheetData>
   <autoFilter ref="A2:O70">
+    <filterColumn colId="3">
+      <filters>
+        <filter val="ID Authentication"/>
+      </filters>
+    </filterColumn>
     <filterColumn colId="8">
       <filters>
         <filter val="1"/>
@@ -7478,12 +7484,12 @@
     </row>
     <row r="8" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B8" s="13" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="9" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B9" s="13" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
     </row>
     <row r="10" spans="2:2" x14ac:dyDescent="0.35">
@@ -7515,13 +7521,13 @@
   <sheetData>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="44" t="s">
+        <v>192</v>
+      </c>
+      <c r="B3" t="s">
+        <v>194</v>
+      </c>
+      <c r="C3" t="s">
         <v>195</v>
-      </c>
-      <c r="B3" t="s">
-        <v>197</v>
-      </c>
-      <c r="C3" t="s">
-        <v>198</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
@@ -7548,7 +7554,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" s="45" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B6" s="46">
         <v>3</v>
@@ -7603,7 +7609,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" s="45" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="B11" s="46">
         <v>64</v>

</xml_diff>

<commit_message>
Updated the Comment and Status for Reg Processor CRs
- Added Legends for CRs
- Updated Mindtree Comments for CRs
- Updated the Current Status of the CRs
</commit_message>
<xml_diff>
--- a/requirements/MOSIP_Requirements Change_Tracker_18Dec18_Updated.xlsx
+++ b/requirements/MOSIP_Requirements Change_Tracker_18Dec18_Updated.xlsx
@@ -1,40 +1,46 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\m1032103\Desktop\PROJECTS\MOSIP\Desk Items\Change Tracker\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\M1045452\Documents\GitHub\mosip\requirements\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{5A105D0B-97B2-412C-9378-401E5AA528B1}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FA7AF68-29A7-4F32-90DB-5D591A089697}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9675" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9680" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MOSIP_QueryLog_External" sheetId="5" r:id="rId1"/>
     <sheet name="Values" sheetId="2" r:id="rId2"/>
     <sheet name="Pivot" sheetId="7" r:id="rId3"/>
+    <sheet name="Status Legends" sheetId="8" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">MOSIP_QueryLog_External!$A$2:$Q$76</definedName>
   </definedNames>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="179021"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId4"/>
+    <pivotCache cacheId="2" r:id="rId5"/>
   </pivotCaches>
   <fileRecoveryPr autoRecover="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="729" uniqueCount="235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="738" uniqueCount="246">
   <si>
     <t>MOSIP - Requirements Change Log</t>
   </si>
@@ -1837,9 +1843,6 @@
     </r>
   </si>
   <si>
-    <t>need to install clamav in private network VM and minor code changes</t>
-  </si>
-  <si>
     <t>Internal requirement evaluation</t>
   </si>
   <si>
@@ -2346,9 +2349,6 @@
     <t>Sprint</t>
   </si>
   <si>
-    <t>Clarity in requirement is needed by Sprint 7, taken up in Sprint 9 as we need API specs</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <u/>
@@ -2496,15 +2496,9 @@
     </r>
   </si>
   <si>
-    <t>Clarity in requirement is needed by Sprint 7, taken up in Sprint 9 as we need API specs for CNIE</t>
-  </si>
-  <si>
     <t>Sprint 10</t>
   </si>
   <si>
-    <t>Process flow diagram on how EC integrates with MOSIP. Clarity in requirement is needed by Sprint 7</t>
-  </si>
-  <si>
     <t>Sprint 7</t>
   </si>
   <si>
@@ -2517,9 +2511,6 @@
     <t>Sprint 8</t>
   </si>
   <si>
-    <t>Resham to confirm with Shrikanth</t>
-  </si>
-  <si>
     <t>Dev Complete</t>
   </si>
   <si>
@@ -2529,14 +2520,7 @@
     <t>Need clarity on requirements</t>
   </si>
   <si>
-    <t xml:space="preserve">Need clarity in requirement as it does not add value (TBD with Shravan) </t>
-  </si>
-  <si>
     <t>Code to be removed</t>
-  </si>
-  <si>
-    <t>As per discussion with Sanjay this is not required.
-We need to Undo Some Changes as it was Implemented in Sprint 6.</t>
   </si>
   <si>
     <t>Dev in progress</t>
@@ -2831,6 +2815,72 @@
       </rPr>
       <t>Place in CR tracker if excluded</t>
     </r>
+  </si>
+  <si>
+    <t>We need API specs to integrate with CNIE.
+We need a Process Flow of the entire CNIE Process.
+Clarity in requirement is needed by Sprint 7, will be taken up in Sprint 9.</t>
+  </si>
+  <si>
+    <t>Process flow diagram on how EC integrates with MOSIP. 
+Clarity in requirement is needed by Sprint 7</t>
+  </si>
+  <si>
+    <t>Dev Not Needed
+Part of Dummy ABIS</t>
+  </si>
+  <si>
+    <t>We are Developing a mock ABIS which will do de-dupe, But Integration will be conducted once GoM provides its ABIS.</t>
+  </si>
+  <si>
+    <t>Dev Not Needed
+(De-Scoped)</t>
+  </si>
+  <si>
+    <t>We will Provide a Hook for Integration.
+The below will require a code change to be carried out by the SI
+i. Add the Country's Manual Verification Layer and 
+ii. Change in Camel Configurations to Add the New Verticel</t>
+  </si>
+  <si>
+    <t>Sprint8</t>
+  </si>
+  <si>
+    <t>As per discussion with Sanjay this is not required.
+We need to Undo Some Changes as it was Implemented in Sprint 6.</t>
+  </si>
+  <si>
+    <t>FIT-2</t>
+  </si>
+  <si>
+    <t>Need to install clamav in private network VM and minor code changes.
+There is a Change in the Process Flow and the same has been updated in the Process Flow Diagram.</t>
+  </si>
+  <si>
+    <t>(Clarified By Shravan)
+We will use a Mapping JSON to identify Packets with Master Data and Validate the Same using Kernel Master Data
+If New Master Data is added there will be Code Changes for this Validation</t>
+  </si>
+  <si>
+    <t>Validation of Packet Created During Working Hours will be taken Up in Sprint 8</t>
+  </si>
+  <si>
+    <t>Clarification on the Requierment is Not Clear</t>
+  </si>
+  <si>
+    <t>Requierment Clarified - Dev In Progress/Completed</t>
+  </si>
+  <si>
+    <t>Requierment Clarified - Dev Yet to Start</t>
+  </si>
+  <si>
+    <t>Requierment is De-Scoped</t>
+  </si>
+  <si>
+    <t>Color</t>
+  </si>
+  <si>
+    <t>Description</t>
   </si>
 </sst>
 </file>
@@ -2840,7 +2890,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0;[Red]0"/>
   </numFmts>
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2924,8 +2974,16 @@
       <name val="Cambria"/>
       <family val="1"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2958,12 +3016,36 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -3049,12 +3131,51 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="71">
+  <cellXfs count="83">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -3203,9 +3324,6 @@
     <xf numFmtId="2" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3224,9 +3342,6 @@
     <xf numFmtId="15" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3239,9 +3354,6 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3253,6 +3365,51 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -4462,7 +4619,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0200-000000000000}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0200-000000000000}" name="PivotTable1" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:C11" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="15">
     <pivotField dataField="1" showAll="0"/>
@@ -4814,55 +4971,55 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:S78"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A73" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A77" sqref="A77"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="20.28515625" defaultRowHeight="14.25" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="20.26953125" defaultRowHeight="14" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="6.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.453125" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14" style="2" customWidth="1"/>
-    <col min="3" max="3" width="30.42578125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="15.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.7109375" style="3" customWidth="1"/>
-    <col min="6" max="6" width="71.140625" style="3" customWidth="1"/>
-    <col min="7" max="7" width="13.28515625" style="17" customWidth="1"/>
-    <col min="8" max="8" width="44.42578125" style="3" customWidth="1"/>
-    <col min="9" max="9" width="9.28515625" style="3" customWidth="1"/>
-    <col min="10" max="10" width="20.85546875" style="3" customWidth="1"/>
-    <col min="11" max="11" width="12.28515625" style="3" customWidth="1"/>
-    <col min="12" max="12" width="12.5703125" style="3" customWidth="1"/>
-    <col min="13" max="13" width="12.140625" style="29" hidden="1" customWidth="1"/>
-    <col min="14" max="14" width="15.85546875" style="2" customWidth="1"/>
-    <col min="15" max="15" width="15.85546875" style="11" customWidth="1"/>
-    <col min="16" max="16" width="15.85546875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="30.453125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="15.7265625" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.7265625" style="3" customWidth="1"/>
+    <col min="6" max="6" width="71.1796875" style="3" customWidth="1"/>
+    <col min="7" max="7" width="13.26953125" style="17" customWidth="1"/>
+    <col min="8" max="8" width="44.453125" style="3" customWidth="1"/>
+    <col min="9" max="9" width="9.26953125" style="3" customWidth="1"/>
+    <col min="10" max="10" width="20.81640625" style="3" customWidth="1"/>
+    <col min="11" max="11" width="12.26953125" style="3" customWidth="1"/>
+    <col min="12" max="12" width="12.54296875" style="3" customWidth="1"/>
+    <col min="13" max="13" width="12.1796875" style="29" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="15.81640625" style="2" customWidth="1"/>
+    <col min="15" max="15" width="15.81640625" style="11" customWidth="1"/>
+    <col min="16" max="16" width="15.81640625" style="2" customWidth="1"/>
     <col min="17" max="17" width="35" style="3" customWidth="1"/>
-    <col min="18" max="16384" width="20.28515625" style="11"/>
+    <col min="18" max="16384" width="20.26953125" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="67" t="s">
+    <row r="1" spans="1:17" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="64" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="68"/>
-      <c r="C1" s="68"/>
-      <c r="D1" s="68"/>
-      <c r="E1" s="68"/>
-      <c r="F1" s="68"/>
-      <c r="G1" s="68"/>
-      <c r="H1" s="68"/>
-      <c r="I1" s="68"/>
-      <c r="J1" s="68"/>
-      <c r="K1" s="68"/>
-      <c r="L1" s="68"/>
-      <c r="M1" s="68"/>
-      <c r="N1" s="68"/>
-      <c r="O1" s="69"/>
-      <c r="P1" s="68"/>
-      <c r="Q1" s="70"/>
-    </row>
-    <row r="2" spans="1:17" ht="57" x14ac:dyDescent="0.25">
+      <c r="B1" s="65"/>
+      <c r="C1" s="65"/>
+      <c r="D1" s="65"/>
+      <c r="E1" s="65"/>
+      <c r="F1" s="65"/>
+      <c r="G1" s="65"/>
+      <c r="H1" s="65"/>
+      <c r="I1" s="65"/>
+      <c r="J1" s="65"/>
+      <c r="K1" s="65"/>
+      <c r="L1" s="65"/>
+      <c r="M1" s="65"/>
+      <c r="N1" s="65"/>
+      <c r="O1" s="66"/>
+      <c r="P1" s="65"/>
+      <c r="Q1" s="67"/>
+    </row>
+    <row r="2" spans="1:17" ht="42" x14ac:dyDescent="0.35">
       <c r="A2" s="19" t="s">
         <v>1</v>
       </c>
@@ -4900,22 +5057,22 @@
         <v>12</v>
       </c>
       <c r="M2" s="26" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="N2" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="O2" s="64" t="s">
+      <c r="O2" s="62" t="s">
+        <v>207</v>
+      </c>
+      <c r="P2" s="21" t="s">
         <v>208</v>
-      </c>
-      <c r="P2" s="21" t="s">
-        <v>209</v>
       </c>
       <c r="Q2" s="21" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:17" s="4" customFormat="1" ht="128.25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" s="4" customFormat="1" ht="112" hidden="1" x14ac:dyDescent="0.35">
       <c r="A3" s="5">
         <v>1</v>
       </c>
@@ -4956,7 +5113,7 @@
         <v>36</v>
       </c>
       <c r="N3" s="32" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="O3" s="32"/>
       <c r="P3" s="32"/>
@@ -4964,7 +5121,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:17" s="4" customFormat="1" ht="57" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" s="4" customFormat="1" ht="56" hidden="1" x14ac:dyDescent="0.35">
       <c r="A4" s="5">
         <v>2</v>
       </c>
@@ -5013,7 +5170,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:17" s="4" customFormat="1" ht="71.25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" s="4" customFormat="1" ht="70" hidden="1" x14ac:dyDescent="0.35">
       <c r="A5" s="5">
         <v>3</v>
       </c>
@@ -5054,7 +5211,7 @@
         <v>35</v>
       </c>
       <c r="N5" s="32" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="O5" s="32"/>
       <c r="P5" s="32"/>
@@ -5062,7 +5219,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:17" s="4" customFormat="1" ht="57" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" s="4" customFormat="1" ht="56" hidden="1" x14ac:dyDescent="0.35">
       <c r="A6" s="5">
         <v>4</v>
       </c>
@@ -5103,7 +5260,7 @@
         <v>30</v>
       </c>
       <c r="N6" s="32" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="O6" s="32"/>
       <c r="P6" s="32"/>
@@ -5111,7 +5268,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:17" s="1" customFormat="1" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:17" s="1" customFormat="1" ht="42" hidden="1" x14ac:dyDescent="0.3">
       <c r="A7" s="5">
         <v>5</v>
       </c>
@@ -5152,13 +5309,13 @@
         <v>0</v>
       </c>
       <c r="N7" s="32" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="O7" s="32"/>
       <c r="P7" s="32"/>
       <c r="Q7" s="22"/>
     </row>
-    <row r="8" spans="1:17" s="1" customFormat="1" ht="57" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:17" s="1" customFormat="1" ht="56" hidden="1" x14ac:dyDescent="0.3">
       <c r="A8" s="5">
         <v>6</v>
       </c>
@@ -5199,13 +5356,13 @@
         <v>36</v>
       </c>
       <c r="N8" s="32" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="O8" s="32"/>
       <c r="P8" s="32"/>
       <c r="Q8" s="22"/>
     </row>
-    <row r="9" spans="1:17" s="1" customFormat="1" ht="213.75" hidden="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:17" s="1" customFormat="1" ht="210" hidden="1" x14ac:dyDescent="0.3">
       <c r="A9" s="5">
         <v>7</v>
       </c>
@@ -5251,7 +5408,7 @@
       <c r="P9" s="32"/>
       <c r="Q9" s="22"/>
     </row>
-    <row r="10" spans="1:17" s="1" customFormat="1" ht="71.25" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:17" s="1" customFormat="1" ht="56" hidden="1" x14ac:dyDescent="0.3">
       <c r="A10" s="5">
         <v>8</v>
       </c>
@@ -5292,7 +5449,7 @@
         <v>20</v>
       </c>
       <c r="N10" s="32" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="O10" s="32"/>
       <c r="P10" s="32"/>
@@ -5300,7 +5457,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="11" spans="1:17" s="1" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:17" s="1" customFormat="1" ht="120" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="5">
         <v>9</v>
       </c>
@@ -5316,8 +5473,8 @@
       <c r="E11" s="34" t="s">
         <v>32</v>
       </c>
-      <c r="F11" s="56" t="s">
-        <v>212</v>
+      <c r="F11" s="55" t="s">
+        <v>210</v>
       </c>
       <c r="G11" s="15" t="s">
         <v>46</v>
@@ -5337,23 +5494,23 @@
       <c r="L11" s="22">
         <v>43419</v>
       </c>
-      <c r="M11" s="55" t="s">
+      <c r="M11" s="54" t="s">
         <v>50</v>
       </c>
       <c r="N11" s="43">
         <v>36</v>
       </c>
-      <c r="O11" s="65" t="s">
+      <c r="O11" s="68" t="s">
+        <v>202</v>
+      </c>
+      <c r="P11" s="32" t="s">
         <v>203</v>
       </c>
-      <c r="P11" s="32" t="s">
-        <v>204</v>
-      </c>
       <c r="Q11" s="22" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17" s="1" customFormat="1" ht="128.25" x14ac:dyDescent="0.2">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" s="1" customFormat="1" ht="126.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="5">
         <v>10</v>
       </c>
@@ -5369,8 +5526,8 @@
       <c r="E12" s="34" t="s">
         <v>32</v>
       </c>
-      <c r="F12" s="56" t="s">
-        <v>211</v>
+      <c r="F12" s="55" t="s">
+        <v>209</v>
       </c>
       <c r="G12" s="15" t="s">
         <v>46</v>
@@ -5390,23 +5547,23 @@
       <c r="L12" s="22">
         <v>43419</v>
       </c>
-      <c r="M12" s="57">
+      <c r="M12" s="56">
         <v>36</v>
       </c>
       <c r="N12" s="43">
         <v>54</v>
       </c>
-      <c r="O12" s="65" t="s">
+      <c r="O12" s="68" t="s">
+        <v>202</v>
+      </c>
+      <c r="P12" s="32" t="s">
         <v>203</v>
       </c>
-      <c r="P12" s="32" t="s">
-        <v>204</v>
-      </c>
       <c r="Q12" s="22" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="13" spans="1:17" s="4" customFormat="1" ht="171" x14ac:dyDescent="0.25">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" s="4" customFormat="1" ht="154" x14ac:dyDescent="0.35">
       <c r="A13" s="5">
         <v>11</v>
       </c>
@@ -5443,23 +5600,23 @@
       <c r="L13" s="22">
         <v>43419</v>
       </c>
-      <c r="M13" s="55" t="s">
+      <c r="M13" s="54" t="s">
         <v>55</v>
       </c>
       <c r="N13" s="43">
         <v>72</v>
       </c>
-      <c r="O13" s="65" t="s">
-        <v>203</v>
+      <c r="O13" s="68" t="s">
+        <v>202</v>
       </c>
       <c r="P13" s="32" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="Q13" s="22" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17" s="1" customFormat="1" ht="114" x14ac:dyDescent="0.2">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" s="1" customFormat="1" ht="98" x14ac:dyDescent="0.3">
       <c r="A14" s="5">
         <v>12</v>
       </c>
@@ -5502,17 +5659,17 @@
       <c r="N14" s="43">
         <v>0</v>
       </c>
-      <c r="O14" s="65" t="s">
-        <v>203</v>
+      <c r="O14" s="69" t="s">
+        <v>230</v>
       </c>
       <c r="P14" s="32" t="s">
-        <v>216</v>
+        <v>186</v>
       </c>
       <c r="Q14" s="22" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="15" spans="1:17" s="4" customFormat="1" ht="114" x14ac:dyDescent="0.25">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" s="4" customFormat="1" ht="98" x14ac:dyDescent="0.35">
       <c r="A15" s="5">
         <v>13</v>
       </c>
@@ -5549,23 +5706,23 @@
       <c r="L15" s="22">
         <v>43419</v>
       </c>
-      <c r="M15" s="58">
+      <c r="M15" s="57">
         <v>10</v>
       </c>
-      <c r="N15" s="59" t="s">
-        <v>218</v>
-      </c>
-      <c r="O15" s="65" t="s">
-        <v>203</v>
-      </c>
-      <c r="P15" s="59" t="s">
-        <v>219</v>
-      </c>
-      <c r="Q15" s="60" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="16" spans="1:17" s="1" customFormat="1" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="N15" s="58" t="s">
+        <v>214</v>
+      </c>
+      <c r="O15" s="70" t="s">
+        <v>202</v>
+      </c>
+      <c r="P15" s="58" t="s">
+        <v>215</v>
+      </c>
+      <c r="Q15" s="59" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" s="1" customFormat="1" ht="42" hidden="1" x14ac:dyDescent="0.3">
       <c r="A16" s="5">
         <v>14</v>
       </c>
@@ -5606,7 +5763,7 @@
       <c r="P16" s="32"/>
       <c r="Q16" s="22"/>
     </row>
-    <row r="17" spans="1:17" s="4" customFormat="1" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17" s="4" customFormat="1" ht="42" hidden="1" x14ac:dyDescent="0.35">
       <c r="A17" s="5">
         <v>15</v>
       </c>
@@ -5647,7 +5804,7 @@
       <c r="P17" s="32"/>
       <c r="Q17" s="22"/>
     </row>
-    <row r="18" spans="1:17" ht="99.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:17" ht="84" hidden="1" x14ac:dyDescent="0.35">
       <c r="A18" s="5">
         <v>16</v>
       </c>
@@ -5696,7 +5853,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="19" spans="1:17" ht="99.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:17" ht="84" hidden="1" x14ac:dyDescent="0.35">
       <c r="A19" s="5">
         <v>17</v>
       </c>
@@ -5737,7 +5894,7 @@
         <v>5</v>
       </c>
       <c r="N19" s="32" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="O19" s="32"/>
       <c r="P19" s="32"/>
@@ -5745,7 +5902,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="20" spans="1:17" ht="99.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:17" ht="84" x14ac:dyDescent="0.35">
       <c r="A20" s="5">
         <v>18</v>
       </c>
@@ -5782,23 +5939,23 @@
       <c r="L20" s="22">
         <v>43419</v>
       </c>
-      <c r="M20" s="57">
+      <c r="M20" s="56">
         <v>20</v>
       </c>
       <c r="N20" s="43">
         <v>30</v>
       </c>
-      <c r="O20" s="65" t="s">
-        <v>203</v>
+      <c r="O20" s="70" t="s">
+        <v>202</v>
       </c>
       <c r="P20" s="32" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="Q20" s="22" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="21" spans="1:17" ht="85.5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:17" ht="84" hidden="1" x14ac:dyDescent="0.35">
       <c r="A21" s="5">
         <v>19</v>
       </c>
@@ -5841,7 +5998,7 @@
       <c r="P21" s="32"/>
       <c r="Q21" s="22"/>
     </row>
-    <row r="22" spans="1:17" ht="99.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:17" ht="84" hidden="1" x14ac:dyDescent="0.35">
       <c r="A22" s="5">
         <v>20</v>
       </c>
@@ -5884,7 +6041,7 @@
       <c r="P22" s="32"/>
       <c r="Q22" s="22"/>
     </row>
-    <row r="23" spans="1:17" ht="99.75" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:17" ht="84" hidden="1" x14ac:dyDescent="0.35">
       <c r="A23" s="5">
         <v>21</v>
       </c>
@@ -5933,7 +6090,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="24" spans="1:17" ht="85.5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:17" ht="84" hidden="1" x14ac:dyDescent="0.35">
       <c r="A24" s="5">
         <v>22</v>
       </c>
@@ -5974,7 +6131,7 @@
         <v>5</v>
       </c>
       <c r="N24" s="32" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="O24" s="32"/>
       <c r="P24" s="32"/>
@@ -5982,7 +6139,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="25" spans="1:17" ht="85.5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:17" ht="84" hidden="1" x14ac:dyDescent="0.35">
       <c r="A25" s="5">
         <v>23</v>
       </c>
@@ -6025,7 +6182,7 @@
       <c r="P25" s="32"/>
       <c r="Q25" s="22"/>
     </row>
-    <row r="26" spans="1:17" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:17" ht="42" hidden="1" x14ac:dyDescent="0.35">
       <c r="A26" s="5">
         <v>24</v>
       </c>
@@ -6066,13 +6223,13 @@
         <v>30</v>
       </c>
       <c r="N26" s="32" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="O26" s="32"/>
       <c r="P26" s="32"/>
       <c r="Q26" s="15"/>
     </row>
-    <row r="27" spans="1:17" ht="85.5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:17" ht="84" x14ac:dyDescent="0.35">
       <c r="A27" s="5">
         <v>25</v>
       </c>
@@ -6109,23 +6266,23 @@
       <c r="L27" s="22">
         <v>43419</v>
       </c>
-      <c r="M27" s="57">
+      <c r="M27" s="56">
         <v>20</v>
       </c>
       <c r="N27" s="43">
         <v>30</v>
       </c>
-      <c r="O27" s="65" t="s">
-        <v>221</v>
+      <c r="O27" s="71" t="s">
+        <v>216</v>
       </c>
       <c r="P27" s="32" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="Q27" s="15" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="28" spans="1:17" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:17" ht="42" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="5">
         <v>26</v>
       </c>
@@ -6142,7 +6299,7 @@
         <v>32</v>
       </c>
       <c r="F28" s="20" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="G28" s="15" t="s">
         <v>46</v>
@@ -6166,13 +6323,13 @@
         <v>6</v>
       </c>
       <c r="N28" s="32" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="O28" s="32"/>
       <c r="P28" s="32"/>
       <c r="Q28" s="34"/>
     </row>
-    <row r="29" spans="1:17" s="8" customFormat="1" ht="85.5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:17" s="8" customFormat="1" ht="84" hidden="1" x14ac:dyDescent="0.35">
       <c r="A29" s="5">
         <v>27</v>
       </c>
@@ -6221,7 +6378,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="30" spans="1:17" s="8" customFormat="1" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:17" s="8" customFormat="1" ht="42" hidden="1" x14ac:dyDescent="0.35">
       <c r="A30" s="5">
         <v>28</v>
       </c>
@@ -6270,7 +6427,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="31" spans="1:17" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:17" ht="42" hidden="1" x14ac:dyDescent="0.35">
       <c r="A31" s="5">
         <v>29</v>
       </c>
@@ -6311,13 +6468,13 @@
         <v>1</v>
       </c>
       <c r="N31" s="32" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="O31" s="32"/>
       <c r="P31" s="32"/>
       <c r="Q31" s="15"/>
     </row>
-    <row r="32" spans="1:17" ht="128.25" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:17" ht="126" hidden="1" x14ac:dyDescent="0.35">
       <c r="A32" s="5">
         <v>30</v>
       </c>
@@ -6358,7 +6515,7 @@
         <v>0</v>
       </c>
       <c r="N32" s="32" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="O32" s="32"/>
       <c r="P32" s="32"/>
@@ -6366,7 +6523,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="33" spans="1:17" ht="71.25" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:17" ht="70" hidden="1" x14ac:dyDescent="0.35">
       <c r="A33" s="5">
         <v>31</v>
       </c>
@@ -6412,10 +6569,10 @@
       <c r="O33" s="32"/>
       <c r="P33" s="32"/>
       <c r="Q33" s="34" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="34" spans="1:17" ht="142.5" x14ac:dyDescent="0.25">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="34" spans="1:17" ht="140" hidden="1" x14ac:dyDescent="0.35">
       <c r="A34" s="5">
         <v>32</v>
       </c>
@@ -6456,15 +6613,15 @@
         <v>0</v>
       </c>
       <c r="N34" s="32" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="O34" s="32"/>
       <c r="P34" s="32"/>
       <c r="Q34" s="34" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="35" spans="1:17" ht="71.25" x14ac:dyDescent="0.25">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="35" spans="1:17" ht="70" hidden="1" x14ac:dyDescent="0.35">
       <c r="A35" s="5">
         <v>33</v>
       </c>
@@ -6505,15 +6662,15 @@
         <v>0</v>
       </c>
       <c r="N35" s="32" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="O35" s="32"/>
       <c r="P35" s="32"/>
       <c r="Q35" s="34" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="36" spans="1:17" ht="36" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="36" spans="1:17" ht="36" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" s="5">
         <v>34</v>
       </c>
@@ -6556,7 +6713,7 @@
       <c r="P36" s="32"/>
       <c r="Q36" s="34"/>
     </row>
-    <row r="37" spans="1:17" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:17" ht="28" hidden="1" x14ac:dyDescent="0.35">
       <c r="A37" s="5">
         <v>35</v>
       </c>
@@ -6602,7 +6759,7 @@
       <c r="P37" s="32"/>
       <c r="Q37" s="34"/>
     </row>
-    <row r="38" spans="1:17" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:17" ht="28" hidden="1" x14ac:dyDescent="0.35">
       <c r="A38" s="5">
         <v>36</v>
       </c>
@@ -6628,7 +6785,7 @@
         <v>118</v>
       </c>
       <c r="I38" s="34" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="J38" s="34" t="s">
         <v>87</v>
@@ -6650,7 +6807,7 @@
       <c r="P38" s="32"/>
       <c r="Q38" s="34"/>
     </row>
-    <row r="39" spans="1:17" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:17" ht="28" hidden="1" x14ac:dyDescent="0.35">
       <c r="A39" s="5">
         <v>37</v>
       </c>
@@ -6696,7 +6853,7 @@
       <c r="P39" s="32"/>
       <c r="Q39" s="34"/>
     </row>
-    <row r="40" spans="1:17" ht="256.5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:17" ht="252" hidden="1" x14ac:dyDescent="0.35">
       <c r="A40" s="5">
         <v>38</v>
       </c>
@@ -6722,7 +6879,7 @@
         <v>121</v>
       </c>
       <c r="I40" s="34" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="J40" s="34" t="s">
         <v>87</v>
@@ -6733,21 +6890,21 @@
       <c r="L40" s="22">
         <v>43440</v>
       </c>
-      <c r="M40" s="57">
+      <c r="M40" s="56">
         <v>60</v>
       </c>
       <c r="N40" s="43">
         <v>90</v>
       </c>
-      <c r="O40" s="65" t="s">
-        <v>203</v>
+      <c r="O40" s="63" t="s">
+        <v>202</v>
       </c>
       <c r="P40" s="32"/>
       <c r="Q40" s="34" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="41" spans="1:17" ht="99.75" hidden="1" x14ac:dyDescent="0.25">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="41" spans="1:17" ht="98" hidden="1" x14ac:dyDescent="0.35">
       <c r="A41" s="5">
         <v>40</v>
       </c>
@@ -6794,7 +6951,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="42" spans="1:17" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:17" ht="56" x14ac:dyDescent="0.35">
       <c r="A42" s="5">
         <v>41</v>
       </c>
@@ -6837,17 +6994,17 @@
       <c r="N42" s="32" t="s">
         <v>52</v>
       </c>
-      <c r="O42" s="65" t="s">
-        <v>227</v>
+      <c r="O42" s="71" t="s">
+        <v>220</v>
       </c>
       <c r="P42" s="32" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="Q42" s="34" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="43" spans="1:17" ht="28.5" x14ac:dyDescent="0.25">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="43" spans="1:17" ht="116" x14ac:dyDescent="0.35">
       <c r="A43" s="5">
         <v>42</v>
       </c>
@@ -6864,7 +7021,7 @@
         <v>32</v>
       </c>
       <c r="F43" s="20" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="G43" s="15" t="s">
         <v>46</v>
@@ -6890,17 +7047,17 @@
       <c r="N43" s="43">
         <v>30</v>
       </c>
-      <c r="O43" s="65" t="s">
-        <v>203</v>
+      <c r="O43" s="69" t="s">
+        <v>232</v>
       </c>
       <c r="P43" s="32" t="s">
-        <v>219</v>
-      </c>
-      <c r="Q43" s="61" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="44" spans="1:17" ht="57" hidden="1" x14ac:dyDescent="0.25">
+        <v>186</v>
+      </c>
+      <c r="Q43" s="72" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="44" spans="1:17" ht="56" hidden="1" x14ac:dyDescent="0.35">
       <c r="A44" s="5">
         <v>45</v>
       </c>
@@ -6917,13 +7074,13 @@
         <v>32</v>
       </c>
       <c r="F44" s="20" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="G44" s="15" t="s">
         <v>46</v>
       </c>
       <c r="H44" s="34" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="I44" s="34">
         <v>2</v>
@@ -6932,7 +7089,7 @@
         <v>87</v>
       </c>
       <c r="K44" s="34" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="L44" s="22">
         <v>43452</v>
@@ -6943,7 +7100,7 @@
       <c r="P44" s="32"/>
       <c r="Q44" s="34"/>
     </row>
-    <row r="45" spans="1:17" ht="57" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:17" ht="70" x14ac:dyDescent="0.35">
       <c r="A45" s="5">
         <v>46</v>
       </c>
@@ -6980,21 +7137,23 @@
       <c r="L45" s="22">
         <v>43440</v>
       </c>
-      <c r="M45" s="62">
+      <c r="M45" s="60">
         <v>5</v>
       </c>
-      <c r="N45" s="63">
+      <c r="N45" s="61">
         <v>8</v>
       </c>
-      <c r="O45" s="66" t="s">
-        <v>225</v>
-      </c>
-      <c r="P45" s="59"/>
+      <c r="O45" s="73" t="s">
+        <v>219</v>
+      </c>
+      <c r="P45" s="58" t="s">
+        <v>234</v>
+      </c>
       <c r="Q45" s="20" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="46" spans="1:17" ht="57" x14ac:dyDescent="0.25">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="46" spans="1:17" ht="56" hidden="1" x14ac:dyDescent="0.35">
       <c r="A46" s="5">
         <v>47</v>
       </c>
@@ -7035,7 +7194,7 @@
         <v>0</v>
       </c>
       <c r="N46" s="32" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="O46" s="32"/>
       <c r="P46" s="32"/>
@@ -7043,7 +7202,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="47" spans="1:17" ht="42.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:17" ht="42" hidden="1" x14ac:dyDescent="0.35">
       <c r="A47" s="5">
         <v>48</v>
       </c>
@@ -7089,7 +7248,7 @@
       <c r="P47" s="32"/>
       <c r="Q47" s="34"/>
     </row>
-    <row r="48" spans="1:17" ht="156.75" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:17" ht="140" hidden="1" x14ac:dyDescent="0.35">
       <c r="A48" s="5">
         <v>49</v>
       </c>
@@ -7132,7 +7291,7 @@
       <c r="P48" s="32"/>
       <c r="Q48" s="34"/>
     </row>
-    <row r="49" spans="1:17" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:17" ht="42" hidden="1" x14ac:dyDescent="0.35">
       <c r="A49" s="5">
         <v>50</v>
       </c>
@@ -7181,7 +7340,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="50" spans="1:17" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:17" ht="42" hidden="1" x14ac:dyDescent="0.35">
       <c r="A50" s="5">
         <v>51</v>
       </c>
@@ -7224,7 +7383,7 @@
       <c r="P50" s="32"/>
       <c r="Q50" s="34"/>
     </row>
-    <row r="51" spans="1:17" ht="28.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:17" ht="28" hidden="1" x14ac:dyDescent="0.35">
       <c r="A51" s="5">
         <v>52</v>
       </c>
@@ -7270,7 +7429,7 @@
       <c r="P51" s="32"/>
       <c r="Q51" s="34"/>
     </row>
-    <row r="52" spans="1:17" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:17" ht="42" hidden="1" x14ac:dyDescent="0.35">
       <c r="A52" s="5">
         <v>53</v>
       </c>
@@ -7287,7 +7446,7 @@
         <v>32</v>
       </c>
       <c r="F52" s="20" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="G52" s="15" t="s">
         <v>46</v>
@@ -7311,7 +7470,7 @@
         <v>20</v>
       </c>
       <c r="N52" s="32" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="O52" s="32"/>
       <c r="P52" s="32"/>
@@ -7319,7 +7478,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="53" spans="1:17" ht="85.5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:17" ht="84" hidden="1" x14ac:dyDescent="0.35">
       <c r="A53" s="5">
         <v>54</v>
       </c>
@@ -7360,7 +7519,7 @@
         <v>40</v>
       </c>
       <c r="N53" s="32" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="O53" s="32"/>
       <c r="P53" s="32"/>
@@ -7368,7 +7527,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="54" spans="1:17" ht="42.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:17" ht="42" hidden="1" x14ac:dyDescent="0.35">
       <c r="A54" s="5">
         <v>55</v>
       </c>
@@ -7414,7 +7573,7 @@
       <c r="P54" s="32"/>
       <c r="Q54" s="34"/>
     </row>
-    <row r="55" spans="1:17" ht="57" hidden="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:17" ht="56" hidden="1" x14ac:dyDescent="0.35">
       <c r="A55" s="5">
         <v>56</v>
       </c>
@@ -7460,7 +7619,7 @@
       <c r="P55" s="32"/>
       <c r="Q55" s="34"/>
     </row>
-    <row r="56" spans="1:17" ht="71.25" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:17" ht="70" hidden="1" x14ac:dyDescent="0.35">
       <c r="A56" s="5">
         <v>57</v>
       </c>
@@ -7501,13 +7660,13 @@
         <v>4</v>
       </c>
       <c r="N56" s="32" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="O56" s="32"/>
       <c r="P56" s="32"/>
       <c r="Q56" s="34"/>
     </row>
-    <row r="57" spans="1:17" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:17" ht="42" hidden="1" x14ac:dyDescent="0.35">
       <c r="A57" s="5">
         <v>58</v>
       </c>
@@ -7556,7 +7715,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="58" spans="1:17" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:17" ht="84" x14ac:dyDescent="0.35">
       <c r="A58" s="5">
         <v>59</v>
       </c>
@@ -7599,17 +7758,17 @@
       <c r="N58" s="43">
         <v>30</v>
       </c>
-      <c r="O58" s="65" t="s">
-        <v>221</v>
+      <c r="O58" s="71" t="s">
+        <v>216</v>
       </c>
       <c r="P58" s="32" t="s">
-        <v>216</v>
+        <v>236</v>
       </c>
       <c r="Q58" s="34" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="59" spans="1:17" ht="99.75" hidden="1" x14ac:dyDescent="0.25">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="59" spans="1:17" ht="84" hidden="1" x14ac:dyDescent="0.35">
       <c r="A59" s="5">
         <v>60</v>
       </c>
@@ -7617,7 +7776,7 @@
         <v>43432</v>
       </c>
       <c r="C59" s="34" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D59" s="34" t="s">
         <v>145</v>
@@ -7626,13 +7785,13 @@
         <v>40</v>
       </c>
       <c r="F59" s="20" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="G59" s="15" t="s">
         <v>46</v>
       </c>
       <c r="H59" s="34" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="I59" s="34">
         <v>2</v>
@@ -7652,7 +7811,7 @@
       <c r="P59" s="35"/>
       <c r="Q59" s="34"/>
     </row>
-    <row r="60" spans="1:17" ht="57" hidden="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:17" ht="56" hidden="1" x14ac:dyDescent="0.35">
       <c r="A60" s="5">
         <v>61</v>
       </c>
@@ -7660,7 +7819,7 @@
         <v>43432</v>
       </c>
       <c r="C60" s="34" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D60" s="34" t="s">
         <v>145</v>
@@ -7669,16 +7828,16 @@
         <v>40</v>
       </c>
       <c r="F60" s="20" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="G60" s="15" t="s">
         <v>46</v>
       </c>
       <c r="H60" s="34" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="I60" s="34" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="J60" s="34" t="s">
         <v>87</v>
@@ -7695,7 +7854,7 @@
       <c r="P60" s="35"/>
       <c r="Q60" s="34"/>
     </row>
-    <row r="61" spans="1:17" ht="171" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:17" ht="154" hidden="1" x14ac:dyDescent="0.35">
       <c r="A61" s="5">
         <v>62</v>
       </c>
@@ -7703,7 +7862,7 @@
         <v>43440</v>
       </c>
       <c r="C61" s="34" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D61" s="34" t="s">
         <v>39</v>
@@ -7712,7 +7871,7 @@
         <v>32</v>
       </c>
       <c r="F61" s="20" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="G61" s="15" t="s">
         <v>46</v>
@@ -7727,7 +7886,7 @@
         <v>87</v>
       </c>
       <c r="K61" s="34" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="L61" s="22">
         <v>43452</v>
@@ -7741,10 +7900,10 @@
       <c r="O61" s="5"/>
       <c r="P61" s="5"/>
       <c r="Q61" s="34" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="62" spans="1:17" ht="99.75" x14ac:dyDescent="0.25">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="62" spans="1:17" ht="98" hidden="1" x14ac:dyDescent="0.35">
       <c r="A62" s="5">
         <v>63</v>
       </c>
@@ -7752,7 +7911,7 @@
         <v>43440</v>
       </c>
       <c r="C62" s="15" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D62" s="34" t="s">
         <v>16</v>
@@ -7761,7 +7920,7 @@
         <v>32</v>
       </c>
       <c r="F62" s="20" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="G62" s="15" t="s">
         <v>46</v>
@@ -7770,7 +7929,7 @@
         <v>99</v>
       </c>
       <c r="I62" s="34" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="J62" s="34" t="s">
         <v>87</v>
@@ -7790,10 +7949,10 @@
       <c r="O62" s="5"/>
       <c r="P62" s="5"/>
       <c r="Q62" s="34" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="63" spans="1:17" ht="99.75" x14ac:dyDescent="0.25">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="63" spans="1:17" ht="98" hidden="1" x14ac:dyDescent="0.35">
       <c r="A63" s="5">
         <v>64</v>
       </c>
@@ -7801,7 +7960,7 @@
         <v>43440</v>
       </c>
       <c r="C63" s="15" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D63" s="34" t="s">
         <v>93</v>
@@ -7810,7 +7969,7 @@
         <v>32</v>
       </c>
       <c r="F63" s="20" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="G63" s="15" t="s">
         <v>46</v>
@@ -7819,7 +7978,7 @@
         <v>99</v>
       </c>
       <c r="I63" s="34" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="J63" s="34" t="s">
         <v>87</v>
@@ -7839,10 +7998,10 @@
       <c r="O63" s="5"/>
       <c r="P63" s="5"/>
       <c r="Q63" s="34" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="64" spans="1:17" ht="228" x14ac:dyDescent="0.25">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="64" spans="1:17" ht="210" hidden="1" x14ac:dyDescent="0.35">
       <c r="A64" s="5">
         <v>65</v>
       </c>
@@ -7850,7 +8009,7 @@
         <v>43446</v>
       </c>
       <c r="C64" s="34" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D64" s="34" t="s">
         <v>16</v>
@@ -7859,7 +8018,7 @@
         <v>32</v>
       </c>
       <c r="F64" s="20" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="G64" s="15" t="s">
         <v>46</v>
@@ -7886,10 +8045,10 @@
       <c r="O64" s="5"/>
       <c r="P64" s="5"/>
       <c r="Q64" s="34" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="65" spans="1:19" ht="42.75" x14ac:dyDescent="0.25">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="65" spans="1:19" ht="42" hidden="1" x14ac:dyDescent="0.35">
       <c r="A65" s="5">
         <v>66</v>
       </c>
@@ -7897,7 +8056,7 @@
         <v>43446</v>
       </c>
       <c r="C65" s="34" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D65" s="34" t="s">
         <v>16</v>
@@ -7906,7 +8065,7 @@
         <v>32</v>
       </c>
       <c r="F65" s="20" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G65" s="15" t="s">
         <v>46</v>
@@ -7934,7 +8093,7 @@
       <c r="P65" s="5"/>
       <c r="Q65" s="34"/>
     </row>
-    <row r="66" spans="1:19" ht="106.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:19" ht="106.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A66" s="5">
         <v>67</v>
       </c>
@@ -7942,7 +8101,7 @@
         <v>43451</v>
       </c>
       <c r="C66" s="34" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D66" s="34" t="s">
         <v>16</v>
@@ -7951,7 +8110,7 @@
         <v>32</v>
       </c>
       <c r="F66" s="20" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="G66" s="15" t="s">
         <v>46</v>
@@ -7978,10 +8137,10 @@
       <c r="O66" s="5"/>
       <c r="P66" s="5"/>
       <c r="Q66" s="34" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="67" spans="1:19" ht="114" x14ac:dyDescent="0.25">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="67" spans="1:19" ht="112" hidden="1" x14ac:dyDescent="0.35">
       <c r="A67" s="5">
         <v>68</v>
       </c>
@@ -7989,7 +8148,7 @@
         <v>43451</v>
       </c>
       <c r="C67" s="34" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D67" s="34" t="s">
         <v>93</v>
@@ -7998,7 +8157,7 @@
         <v>32</v>
       </c>
       <c r="F67" s="20" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G67" s="15" t="s">
         <v>46</v>
@@ -8027,12 +8186,12 @@
       <c r="O67" s="5"/>
       <c r="P67" s="5"/>
       <c r="Q67" s="34" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="R67" s="5"/>
       <c r="S67" s="34"/>
     </row>
-    <row r="68" spans="1:19" ht="128.25" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:19" ht="112" hidden="1" x14ac:dyDescent="0.35">
       <c r="A68" s="5">
         <v>69</v>
       </c>
@@ -8040,7 +8199,7 @@
         <v>43451</v>
       </c>
       <c r="C68" s="34" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D68" s="34" t="s">
         <v>16</v>
@@ -8049,7 +8208,7 @@
         <v>32</v>
       </c>
       <c r="F68" s="20" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="G68" s="15" t="s">
         <v>46</v>
@@ -8079,7 +8238,7 @@
       <c r="R68" s="41"/>
       <c r="S68" s="30"/>
     </row>
-    <row r="69" spans="1:19" ht="85.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:19" ht="84" hidden="1" x14ac:dyDescent="0.35">
       <c r="A69" s="5">
         <v>70</v>
       </c>
@@ -8087,7 +8246,7 @@
         <v>43454</v>
       </c>
       <c r="C69" s="34" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D69" s="30" t="s">
         <v>16</v>
@@ -8096,16 +8255,16 @@
         <v>40</v>
       </c>
       <c r="F69" s="34" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="G69" s="16" t="s">
         <v>46</v>
       </c>
       <c r="H69" s="30" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="I69" s="30" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="J69" s="30" t="s">
         <v>87</v>
@@ -8128,7 +8287,7 @@
       <c r="R69" s="5"/>
       <c r="S69" s="34"/>
     </row>
-    <row r="70" spans="1:19" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:19" ht="84" x14ac:dyDescent="0.35">
       <c r="A70" s="5">
         <v>71</v>
       </c>
@@ -8136,7 +8295,7 @@
         <v>43454</v>
       </c>
       <c r="C70" s="30" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D70" s="30" t="s">
         <v>48</v>
@@ -8145,7 +8304,7 @@
         <v>32</v>
       </c>
       <c r="F70" s="3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G70" s="16" t="s">
         <v>46</v>
@@ -8171,15 +8330,17 @@
       <c r="N70" s="41">
         <v>45</v>
       </c>
-      <c r="O70" s="65" t="s">
+      <c r="O70" s="70" t="s">
+        <v>202</v>
+      </c>
+      <c r="P70" s="41" t="s">
         <v>203</v>
       </c>
-      <c r="P70" s="41" t="s">
-        <v>204</v>
-      </c>
-      <c r="Q70" s="54"/>
-    </row>
-    <row r="71" spans="1:19" ht="99.75" x14ac:dyDescent="0.25">
+      <c r="Q70" s="74" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="71" spans="1:19" ht="98" x14ac:dyDescent="0.35">
       <c r="A71" s="5">
         <v>72</v>
       </c>
@@ -8187,7 +8348,7 @@
         <v>43454</v>
       </c>
       <c r="C71" s="34" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D71" s="34" t="s">
         <v>48</v>
@@ -8196,7 +8357,7 @@
         <v>32</v>
       </c>
       <c r="F71" s="34" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="G71" s="15" t="s">
         <v>46</v>
@@ -8222,15 +8383,17 @@
       <c r="N71" s="43">
         <v>15</v>
       </c>
-      <c r="O71" s="65" t="s">
-        <v>203</v>
+      <c r="O71" s="70" t="s">
+        <v>202</v>
       </c>
       <c r="P71" s="5" t="s">
-        <v>204</v>
-      </c>
-      <c r="Q71" s="32"/>
-    </row>
-    <row r="72" spans="1:19" ht="128.25" x14ac:dyDescent="0.25">
+        <v>215</v>
+      </c>
+      <c r="Q71" s="74" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="72" spans="1:19" ht="126" hidden="1" x14ac:dyDescent="0.35">
       <c r="A72" s="5">
         <v>73</v>
       </c>
@@ -8238,7 +8401,7 @@
         <v>43465</v>
       </c>
       <c r="C72" s="34" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D72" s="34" t="s">
         <v>16</v>
@@ -8247,7 +8410,7 @@
         <v>32</v>
       </c>
       <c r="F72" s="34" t="s">
-        <v>230</v>
+        <v>223</v>
       </c>
       <c r="G72" s="15" t="s">
         <v>46</v>
@@ -8262,7 +8425,7 @@
         <v>87</v>
       </c>
       <c r="K72" s="34" t="s">
-        <v>229</v>
+        <v>222</v>
       </c>
       <c r="L72" s="22">
         <v>43465</v>
@@ -8275,7 +8438,7 @@
       <c r="R72" s="5"/>
       <c r="S72" s="34"/>
     </row>
-    <row r="73" spans="1:19" ht="99.75" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:19" ht="84" hidden="1" x14ac:dyDescent="0.35">
       <c r="A73" s="5">
         <v>74</v>
       </c>
@@ -8283,7 +8446,7 @@
         <v>43465</v>
       </c>
       <c r="C73" s="34" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D73" s="34" t="s">
         <v>16</v>
@@ -8292,7 +8455,7 @@
         <v>32</v>
       </c>
       <c r="F73" s="34" t="s">
-        <v>231</v>
+        <v>224</v>
       </c>
       <c r="G73" s="15" t="s">
         <v>46</v>
@@ -8307,7 +8470,7 @@
         <v>87</v>
       </c>
       <c r="K73" s="34" t="s">
-        <v>229</v>
+        <v>222</v>
       </c>
       <c r="L73" s="22">
         <v>43465</v>
@@ -8320,7 +8483,7 @@
       <c r="R73" s="5"/>
       <c r="S73" s="34"/>
     </row>
-    <row r="74" spans="1:19" ht="57" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:19" ht="56" hidden="1" x14ac:dyDescent="0.35">
       <c r="A74" s="5">
         <v>75</v>
       </c>
@@ -8328,7 +8491,7 @@
         <v>43465</v>
       </c>
       <c r="C74" s="34" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D74" s="34" t="s">
         <v>16</v>
@@ -8337,7 +8500,7 @@
         <v>32</v>
       </c>
       <c r="F74" s="34" t="s">
-        <v>232</v>
+        <v>225</v>
       </c>
       <c r="G74" s="15" t="s">
         <v>46</v>
@@ -8352,7 +8515,7 @@
         <v>87</v>
       </c>
       <c r="K74" s="34" t="s">
-        <v>229</v>
+        <v>222</v>
       </c>
       <c r="L74" s="22">
         <v>43465</v>
@@ -8365,7 +8528,7 @@
       <c r="R74" s="5"/>
       <c r="S74" s="34"/>
     </row>
-    <row r="75" spans="1:19" ht="57" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:19" ht="56" hidden="1" x14ac:dyDescent="0.35">
       <c r="A75" s="5">
         <v>76</v>
       </c>
@@ -8373,7 +8536,7 @@
         <v>43465</v>
       </c>
       <c r="C75" s="34" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D75" s="34" t="s">
         <v>16</v>
@@ -8382,7 +8545,7 @@
         <v>32</v>
       </c>
       <c r="F75" s="34" t="s">
-        <v>233</v>
+        <v>226</v>
       </c>
       <c r="G75" s="15" t="s">
         <v>46</v>
@@ -8397,7 +8560,7 @@
         <v>87</v>
       </c>
       <c r="K75" s="34" t="s">
-        <v>229</v>
+        <v>222</v>
       </c>
       <c r="L75" s="22">
         <v>43465</v>
@@ -8410,7 +8573,7 @@
       <c r="R75" s="5"/>
       <c r="S75" s="34"/>
     </row>
-    <row r="76" spans="1:19" ht="142.5" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:19" ht="140" hidden="1" x14ac:dyDescent="0.35">
       <c r="A76" s="5">
         <v>77</v>
       </c>
@@ -8418,7 +8581,7 @@
         <v>43465</v>
       </c>
       <c r="C76" s="34" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D76" s="34" t="s">
         <v>16</v>
@@ -8427,7 +8590,7 @@
         <v>32</v>
       </c>
       <c r="F76" s="34" t="s">
-        <v>234</v>
+        <v>227</v>
       </c>
       <c r="G76" s="15" t="s">
         <v>46</v>
@@ -8442,7 +8605,7 @@
         <v>87</v>
       </c>
       <c r="K76" s="34" t="s">
-        <v>229</v>
+        <v>222</v>
       </c>
       <c r="L76" s="22">
         <v>43465</v>
@@ -8455,18 +8618,22 @@
       <c r="R76" s="5"/>
       <c r="S76" s="34"/>
     </row>
-    <row r="77" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:19" x14ac:dyDescent="0.35">
       <c r="F77" s="52"/>
     </row>
-    <row r="78" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:19" x14ac:dyDescent="0.35">
       <c r="F78" s="52"/>
     </row>
   </sheetData>
   <autoFilter ref="A2:Q76" xr:uid="{00000000-0009-0000-0000-000000000000}">
+    <filterColumn colId="3">
+      <filters>
+        <filter val="Registration Processor"/>
+      </filters>
+    </filterColumn>
     <filterColumn colId="8">
       <filters>
         <filter val="1"/>
-        <filter val="1+"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -8484,52 +8651,52 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="34.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B3" s="12" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B4" s="7" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="5" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B5" s="7" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B6" s="7" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="7" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B7" s="7" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="8" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B8" s="10" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="9" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B9" s="10" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="10" spans="2:2" x14ac:dyDescent="0.25">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="10" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B10" s="10" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="11" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B11" s="10"/>
     </row>
   </sheetData>
@@ -8544,25 +8711,25 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="34.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="34.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="36" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B3" t="s">
+        <v>174</v>
+      </c>
+      <c r="C3" t="s">
         <v>175</v>
       </c>
-      <c r="C3" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="37" t="s">
         <v>85</v>
       </c>
@@ -8573,7 +8740,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="37" t="s">
         <v>39</v>
       </c>
@@ -8584,7 +8751,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" s="37" t="s">
         <v>145</v>
       </c>
@@ -8595,7 +8762,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="37" t="s">
         <v>93</v>
       </c>
@@ -8606,7 +8773,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" s="37" t="s">
         <v>16</v>
       </c>
@@ -8617,7 +8784,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" s="37" t="s">
         <v>48</v>
       </c>
@@ -8628,7 +8795,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" s="37" t="s">
         <v>62</v>
       </c>
@@ -8639,9 +8806,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" s="37" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B11" s="38">
         <v>64</v>
@@ -8656,13 +8823,78 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{980565A9-FF32-4003-94A7-EC77820C1DD0}">
+  <dimension ref="B1:C5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="3" max="3" width="52.1796875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B1" s="75" t="s">
+        <v>244</v>
+      </c>
+      <c r="C1" s="76" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="2" spans="2:3" ht="31" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B2" s="77"/>
+      <c r="C2" s="78" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3" ht="31" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B3" s="79"/>
+      <c r="C3" s="78" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" ht="31" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B4" s="80"/>
+      <c r="C4" s="78" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" ht="31" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B5" s="81"/>
+      <c r="C5" s="82" t="s">
+        <v>243</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <LikesCount xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <Ratings xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <LikedBy xmlns="http://schemas.microsoft.com/sharepoint/v3">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </LikedBy>
+    <RatedBy xmlns="http://schemas.microsoft.com/sharepoint/v3">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </RatedBy>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -8838,32 +9070,26 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <LikesCount xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <Ratings xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <LikedBy xmlns="http://schemas.microsoft.com/sharepoint/v3">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </LikedBy>
-    <RatedBy xmlns="http://schemas.microsoft.com/sharepoint/v3">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </RatedBy>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6B8E61E4-4805-4EED-8CD4-7E0EB2F2E46E}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0212785F-078B-445B-9297-945E33C92ACD}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -8887,17 +9113,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0212785F-078B-445B-9297-945E33C92ACD}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6B8E61E4-4805-4EED-8CD4-7E0EB2F2E46E}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>